<commit_message>
universal holder folder added
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="212">
   <si>
     <t>QTY</t>
   </si>
@@ -152,16 +152,7 @@
     <t> 5.7</t>
   </si>
   <si>
-    <t> Recommended Options</t>
-  </si>
-  <si>
-    <t>Z Adjust Knob</t>
-  </si>
-  <si>
     <t> 2:40</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Qty</t>
@@ -501,12 +492,6 @@
     <t>Foot Bottom</t>
   </si>
   <si>
-    <t>1.61KG</t>
-  </si>
-  <si>
-    <t>131hrs</t>
-  </si>
-  <si>
     <t> :30</t>
   </si>
   <si>
@@ -764,6 +749,30 @@
   <si>
     <t>TKY_MPCNC_UniversalMount_Mk8_slider.stl
 TKY_MPCNC_UniversalMount_Mk8_bracket.stl</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z Knob</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z_Knob.stl</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>IE-Flex_Foot.STL</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>IE_Foot_Bottom.stl</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>IE_Tool_Holder_13mm_25.stl</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -834,25 +843,9 @@
       <name val="Inherit"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
       <strike/>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FF808080"/>
       <name val="Inherit"/>
     </font>
     <font>
@@ -897,8 +890,23 @@
       <name val="Inherit"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Inherit"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -908,12 +916,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9F9F9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,6 +935,16 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="5" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
   </fills>
@@ -1078,7 +1090,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1193,24 +1205,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1226,22 +1223,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -1256,6 +1253,21 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1265,107 +1277,101 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="46" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="20" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2139,15 +2145,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.375" customWidth="1"/>
@@ -2160,7 +2166,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1">
@@ -2192,718 +2198,707 @@
         <v>8</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="54">
+        <v>4</v>
+      </c>
+      <c r="B4" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="57">
+        <v>0.85</v>
+      </c>
+      <c r="H4" s="54">
+        <v>59.3</v>
+      </c>
+      <c r="I4" s="54">
+        <v>234.5</v>
+      </c>
+      <c r="J4" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>190</v>
+      </c>
+      <c r="L4" s="53">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="54">
+        <v>4</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="57">
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="H5" s="54">
+        <v>17.5</v>
+      </c>
+      <c r="I5" s="54">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="J5" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="66" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="53">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="59">
+        <v>4</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="60">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="62">
+        <v>1.0722222222222222</v>
+      </c>
+      <c r="H6" s="59">
+        <v>89.6</v>
+      </c>
+      <c r="I6" s="59">
+        <v>363</v>
+      </c>
+      <c r="J6" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="K6" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="L6" s="53">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="59">
+        <v>4</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="64">
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="H7" s="59">
+        <v>20.8</v>
+      </c>
+      <c r="I7" s="59">
+        <v>83</v>
+      </c>
+      <c r="J7" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="K7" s="67" t="s">
+        <v>192</v>
+      </c>
+      <c r="L7" s="53">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="59">
+        <v>4</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="64">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="H8" s="59">
+        <v>30.8</v>
+      </c>
+      <c r="I8" s="59">
+        <v>123.5</v>
+      </c>
+      <c r="J8" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8" s="67" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="54">
+        <v>2</v>
+      </c>
+      <c r="B9" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="55">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="57">
+        <v>0.25138888888888888</v>
+      </c>
+      <c r="G9" s="57">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="H9" s="54">
+        <v>66</v>
+      </c>
+      <c r="I9" s="54">
+        <v>132</v>
+      </c>
+      <c r="J9" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="54">
+        <v>2</v>
+      </c>
+      <c r="B10" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="54">
+        <v>11</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" s="54">
+        <v>110.6</v>
+      </c>
+      <c r="J10" s="58"/>
+      <c r="K10" s="66" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="54">
+        <v>2</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="57">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="54">
+        <v>105</v>
+      </c>
+      <c r="J11" s="58"/>
+      <c r="K11" s="66" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="59">
+        <v>2</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" s="63"/>
+      <c r="K12" s="68" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="59">
+        <v>1</v>
+      </c>
+      <c r="B13" s="80" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="60">
+        <v>0.6</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="64">
+        <v>0.19930555555555554</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="59">
+        <v>39</v>
+      </c>
+      <c r="J13" s="63"/>
+      <c r="K13" s="67" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="59">
+        <v>1</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="59">
+        <v>1.04</v>
+      </c>
+      <c r="H14" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="59">
+        <v>12</v>
+      </c>
+      <c r="J14" s="63"/>
+      <c r="K14" s="67" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="59">
+        <v>1</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="J15" s="63"/>
+      <c r="K15" s="67" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="81">
+        <v>1</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="83">
+        <v>0.7</v>
+      </c>
+      <c r="D16" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="81" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="81">
+        <v>5.7</v>
+      </c>
+      <c r="J16" s="85"/>
+      <c r="K16" s="86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="54">
+        <v>1</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="55"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="87">
+        <v>2</v>
+      </c>
+      <c r="B18" s="88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="89">
+        <v>0.7</v>
+      </c>
+      <c r="D18" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="92"/>
+      <c r="K18" s="93" t="s">
+        <v>210</v>
+      </c>
+      <c r="L18" s="39"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="59">
+        <v>1</v>
+      </c>
+      <c r="B19" s="80" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="59">
+      <c r="C19" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="73" t="s">
+        <v>185</v>
+      </c>
+      <c r="L19" s="39"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" spans="1:14" ht="33">
+      <c r="A20" s="59">
+        <v>1</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="74" t="s">
+        <v>203</v>
+      </c>
+      <c r="L20" s="39"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" ht="33">
+      <c r="A21" s="59">
+        <v>1</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="60">
+        <v>0.7</v>
+      </c>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="74" t="s">
+        <v>205</v>
+      </c>
+      <c r="L21" s="39"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="54">
         <v>4</v>
       </c>
-      <c r="B4" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="60">
-        <v>0.4</v>
-      </c>
-      <c r="D4" s="61" t="s">
+      <c r="B22" s="79" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="D22" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E22" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="62">
-        <v>0.85</v>
-      </c>
-      <c r="H4" s="59">
-        <v>59.3</v>
-      </c>
-      <c r="I4" s="59">
-        <v>234.5</v>
-      </c>
-      <c r="J4" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="K4" s="74" t="s">
-        <v>195</v>
-      </c>
-      <c r="L4" s="58">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="59">
+      <c r="F22" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="57">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="54">
+        <v>148.1</v>
+      </c>
+      <c r="J22" s="58"/>
+      <c r="K22" s="66" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="54">
         <v>4</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="60">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="61" t="s">
+      <c r="B23" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="D23" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E23" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="62">
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="H5" s="59">
-        <v>17.5</v>
-      </c>
-      <c r="I5" s="59">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="J5" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="K5" s="74" t="s">
-        <v>194</v>
-      </c>
-      <c r="L5" s="58">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="65">
-        <v>4</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="66">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="68">
-        <v>1.0722222222222222</v>
-      </c>
-      <c r="H6" s="65">
-        <v>89.6</v>
-      </c>
-      <c r="I6" s="65">
-        <v>363</v>
-      </c>
-      <c r="J6" s="69" t="s">
-        <v>186</v>
-      </c>
-      <c r="K6" s="75" t="s">
-        <v>196</v>
-      </c>
-      <c r="L6" s="58">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="65">
-        <v>4</v>
-      </c>
-      <c r="B7" s="70" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="71">
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="H7" s="65">
-        <v>20.8</v>
-      </c>
-      <c r="I7" s="65">
-        <v>83</v>
-      </c>
-      <c r="J7" s="69" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" s="75" t="s">
-        <v>197</v>
-      </c>
-      <c r="L7" s="58">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="65">
-        <v>4</v>
-      </c>
-      <c r="B8" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="71">
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="H8" s="65">
-        <v>30.8</v>
-      </c>
-      <c r="I8" s="65">
-        <v>123.5</v>
-      </c>
-      <c r="J8" s="72" t="s">
-        <v>187</v>
-      </c>
-      <c r="K8" s="75" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="59">
-        <v>2</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="60">
-        <v>0.75</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="62">
-        <v>0.25138888888888888</v>
-      </c>
-      <c r="G9" s="62">
-        <v>0.50277777777777777</v>
-      </c>
-      <c r="H9" s="59">
-        <v>66</v>
-      </c>
-      <c r="I9" s="59">
-        <v>132</v>
-      </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="74" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="59">
-        <v>2</v>
-      </c>
-      <c r="B10" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="60">
-        <v>0.7</v>
-      </c>
-      <c r="D10" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="59">
-        <v>11</v>
-      </c>
-      <c r="H10" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="I10" s="59">
-        <v>110.6</v>
-      </c>
-      <c r="J10" s="63"/>
-      <c r="K10" s="74" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="59">
-        <v>2</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="60">
-        <v>0.7</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="62">
-        <v>0.33611111111111108</v>
-      </c>
-      <c r="H11" s="59" t="s">
-        <v>148</v>
-      </c>
-      <c r="I11" s="59">
-        <v>105</v>
-      </c>
-      <c r="J11" s="63"/>
-      <c r="K11" s="74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="65">
-        <v>2</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="66">
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="I12" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="76" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="65">
-        <v>1</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="66">
-        <v>0.6</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="71">
-        <v>0.19930555555555554</v>
-      </c>
-      <c r="H13" s="65" t="s">
-        <v>151</v>
-      </c>
-      <c r="I13" s="65">
-        <v>39</v>
-      </c>
-      <c r="J13" s="69"/>
-      <c r="K13" s="75" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="65">
-        <v>1</v>
-      </c>
-      <c r="B14" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D14" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="65">
-        <v>1.04</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="65">
-        <v>12</v>
-      </c>
-      <c r="J14" s="69"/>
-      <c r="K14" s="75" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="78">
-        <v>1</v>
-      </c>
-      <c r="B15" s="78" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="79">
-        <v>0.7</v>
-      </c>
-      <c r="D15" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="78" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="78" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="78" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="78">
-        <v>5.7</v>
-      </c>
-      <c r="J15" s="81"/>
-      <c r="K15" s="82" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="59">
-        <v>1</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>201</v>
-      </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="61" t="s">
-        <v>200</v>
-      </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="85" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="86">
-        <v>2</v>
-      </c>
-      <c r="B17" s="87" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="88">
-        <v>0.7</v>
-      </c>
-      <c r="D17" s="89" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="86" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="90"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="65">
-        <v>1</v>
-      </c>
-      <c r="B18" s="70" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="91" t="s">
-        <v>190</v>
-      </c>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" ht="33">
-      <c r="A19" s="65">
-        <v>1</v>
-      </c>
-      <c r="B19" s="70" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="92" t="s">
-        <v>208</v>
-      </c>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" ht="33">
-      <c r="A20" s="65">
-        <v>1</v>
-      </c>
-      <c r="B20" s="70" t="s">
+      <c r="F23" s="57">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="G23" s="57">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H23" s="54">
+        <v>31.8</v>
+      </c>
+      <c r="I23" s="54">
+        <v>127.1</v>
+      </c>
+      <c r="J23" s="58"/>
+      <c r="K23" s="66" t="s">
         <v>209</v>
       </c>
-      <c r="C20" s="66">
-        <v>0.7</v>
-      </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67" t="s">
-        <v>188</v>
-      </c>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="92" t="s">
-        <v>210</v>
-      </c>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="93" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="93"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="93"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="93"/>
-    </row>
-    <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="38">
-        <v>1</v>
-      </c>
-      <c r="B23" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G23" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="H23" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="I23" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="J23" s="42"/>
     </row>
     <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="38">
-        <v>4</v>
-      </c>
-      <c r="B24" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="39">
-        <v>0.6</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="41">
-        <v>0.43055555555555558</v>
-      </c>
-      <c r="H24" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="I24" s="38">
-        <v>148.1</v>
-      </c>
-      <c r="J24" s="42"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="38">
-        <v>4</v>
-      </c>
-      <c r="B25" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" s="39">
-        <v>0.6</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="41">
-        <v>9.7222222222222224E-2</v>
-      </c>
-      <c r="G25" s="41">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="H25" s="38">
-        <v>31.8</v>
-      </c>
-      <c r="I25" s="38">
-        <v>127.1</v>
-      </c>
-      <c r="J25" s="42"/>
-    </row>
-    <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="32" t="s">
-        <v>43</v>
-      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="32" t="s">
-        <v>43</v>
-      </c>
+      <c r="I26" s="1"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A22:I22"/>
-  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
@@ -2924,24 +2919,24 @@
     <hyperlink ref="E11" r:id="rId16" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="D12" r:id="rId17" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
     <hyperlink ref="E12" r:id="rId18"/>
-    <hyperlink ref="D17" r:id="rId19" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
-    <hyperlink ref="E17" r:id="rId20"/>
+    <hyperlink ref="D18" r:id="rId19" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
+    <hyperlink ref="E18" r:id="rId20"/>
     <hyperlink ref="D13" r:id="rId21" location="files" display="http://www.thingiverse.com/thing:806241/ - files"/>
     <hyperlink ref="E13" r:id="rId22"/>
     <hyperlink ref="D14" r:id="rId23" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
     <hyperlink ref="E14" r:id="rId24"/>
-    <hyperlink ref="D15" r:id="rId25" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
-    <hyperlink ref="E15" r:id="rId26" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
-    <hyperlink ref="D23" r:id="rId27" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
-    <hyperlink ref="E23" r:id="rId28" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
-    <hyperlink ref="D24" r:id="rId29" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E24" r:id="rId30" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="D25" r:id="rId31" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E25" r:id="rId32" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E18" r:id="rId33" display="http://www.thingiverse.com/thing:1234989"/>
-    <hyperlink ref="E16" r:id="rId34"/>
-    <hyperlink ref="E19" r:id="rId35"/>
-    <hyperlink ref="E20" r:id="rId36"/>
+    <hyperlink ref="D16" r:id="rId25" location="files" display="http://www.thingiverse.com/thing:724999/ - files"/>
+    <hyperlink ref="E16" r:id="rId26" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
+    <hyperlink ref="D22" r:id="rId27" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
+    <hyperlink ref="E22" r:id="rId28" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
+    <hyperlink ref="D23" r:id="rId29" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
+    <hyperlink ref="E23" r:id="rId30" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
+    <hyperlink ref="E19" r:id="rId31" display="http://www.thingiverse.com/thing:1234989"/>
+    <hyperlink ref="E17" r:id="rId32"/>
+    <hyperlink ref="E20" r:id="rId33"/>
+    <hyperlink ref="E21" r:id="rId34"/>
+    <hyperlink ref="D15" r:id="rId35" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
+    <hyperlink ref="E15" r:id="rId36" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
@@ -2966,30 +2961,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" s="27">
         <v>8500</v>
@@ -2998,13 +2993,13 @@
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>49</v>
-      </c>
       <c r="C3" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="28">
         <v>15000</v>
@@ -3013,13 +3008,13 @@
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="28">
         <f>2900*3</f>
@@ -3032,10 +3027,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5" s="28">
         <v>14000</v>
@@ -3047,10 +3042,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" s="28">
         <f>1500*4</f>
@@ -3063,10 +3058,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D7" s="28">
         <f>1500*4</f>
@@ -3079,10 +3074,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D8" s="28">
         <f>6*2000</f>
@@ -3092,13 +3087,13 @@
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="24"/>
@@ -3108,10 +3103,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="28">
         <f>5*15500</f>
@@ -3124,10 +3119,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="24"/>
@@ -3135,7 +3130,7 @@
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="28">
@@ -3152,13 +3147,13 @@
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="24"/>
@@ -3168,20 +3163,20 @@
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="29"/>
@@ -3197,16 +3192,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="20"/>
       <c r="B19" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="23"/>
@@ -3217,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -3228,7 +3223,7 @@
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="20"/>
       <c r="B21" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="23"/>
@@ -3239,10 +3234,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -3252,10 +3247,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
@@ -3265,10 +3260,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
@@ -3329,25 +3324,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -3355,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="27">
@@ -3366,106 +3361,106 @@
       </c>
       <c r="F2" s="23"/>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="28">
         <v>1500</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>164</v>
+      <c r="F3" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="28">
         <v>1500</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>164</v>
+      <c r="F4" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="28">
         <v>1500</v>
       </c>
-      <c r="F5" s="47" t="s">
-        <v>164</v>
+      <c r="F5" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>95</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="28">
         <v>1500</v>
       </c>
-      <c r="F6" s="47" t="s">
-        <v>164</v>
+      <c r="F6" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -3473,175 +3468,175 @@
         <v>28</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="28">
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="F7" s="47" t="s">
-        <v>164</v>
+      <c r="F7" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51">
+      <c r="A8" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="45"/>
+      <c r="E8" s="46">
         <v>1500</v>
       </c>
-      <c r="F8" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>134</v>
+      <c r="F8" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="51">
+      <c r="A9" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="46">
         <v>1500</v>
       </c>
-      <c r="F9" s="52" t="s">
-        <v>164</v>
-      </c>
-      <c r="G9" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="H9" s="53" t="s">
-        <v>134</v>
+      <c r="F9" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="28">
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>164</v>
+      <c r="F10" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H10" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="28">
         <v>1500</v>
       </c>
-      <c r="F11" s="47" t="s">
-        <v>164</v>
+      <c r="F11" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="47"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="47"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="28">
         <v>1500</v>
       </c>
-      <c r="F14" s="47" t="s">
-        <v>164</v>
+      <c r="F14" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -3649,47 +3644,47 @@
         <v>34</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="28">
         <v>3000</v>
       </c>
-      <c r="F15" s="47" t="s">
-        <v>164</v>
+      <c r="F15" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="28">
         <v>1500</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="G16" t="s">
         <v>164</v>
       </c>
-      <c r="G16" t="s">
-        <v>169</v>
-      </c>
       <c r="H16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -3697,28 +3692,28 @@
         <v>36</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="33">
         <v>1500</v>
       </c>
-      <c r="F17" s="48" t="s">
-        <v>164</v>
+      <c r="F17" s="43" t="s">
+        <v>159</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="49" t="s">
-        <v>166</v>
+      <c r="B18" s="44" t="s">
+        <v>161</v>
       </c>
       <c r="E18" s="31">
         <f>SUM(E2:E17)</f>
@@ -3726,22 +3721,22 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="46" t="s">
-        <v>152</v>
+      <c r="B20" s="41" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3749,7 +3744,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C23">
         <v>68</v>
@@ -3768,7 +3763,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C24">
         <v>68</v>
@@ -3783,7 +3778,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C25">
         <v>50</v>
@@ -3804,132 +3799,132 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C27">
         <v>449</v>
       </c>
       <c r="D27" s="8"/>
-      <c r="E27" s="45">
+      <c r="E27" s="40">
         <v>1500</v>
       </c>
       <c r="G27" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="8:11">
-      <c r="H38" s="55"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42" t="s">
+      <c r="H38" s="50"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="K38" s="38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11">
+      <c r="H39" s="76" t="s">
         <v>175</v>
       </c>
-      <c r="K38" s="42" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="8:11">
-      <c r="H39" s="94" t="s">
-        <v>180</v>
-      </c>
-      <c r="I39" s="42" t="s">
-        <v>172</v>
-      </c>
-      <c r="J39" s="55">
+      <c r="I39" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="J39" s="50">
         <v>40</v>
       </c>
-      <c r="K39" s="55">
+      <c r="K39" s="50">
         <f>J39/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="40" spans="8:11">
-      <c r="H40" s="95"/>
-      <c r="I40" s="42" t="s">
-        <v>173</v>
-      </c>
-      <c r="J40" s="55">
+      <c r="H40" s="77"/>
+      <c r="I40" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="J40" s="50">
         <v>40</v>
       </c>
-      <c r="K40" s="55">
+      <c r="K40" s="50">
         <f t="shared" ref="K40:K41" si="1">J40/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="41" spans="8:11">
-      <c r="H41" s="95"/>
-      <c r="I41" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="J41" s="55">
+      <c r="H41" s="77"/>
+      <c r="I41" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J41" s="50">
         <v>25</v>
       </c>
-      <c r="K41" s="55">
+      <c r="K41" s="50">
         <f t="shared" si="1"/>
         <v>9.8425196850393704</v>
       </c>
     </row>
     <row r="42" spans="8:11">
-      <c r="H42" s="56"/>
-      <c r="I42" s="56"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="56"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
     </row>
     <row r="43" spans="8:11">
-      <c r="H43" s="94" t="s">
-        <v>181</v>
-      </c>
-      <c r="I43" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="J43" s="55">
+      <c r="H43" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="I43" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="J43" s="50">
         <f>J39+27</f>
         <v>67</v>
       </c>
-      <c r="K43" s="55">
+      <c r="K43" s="50">
         <f>J43/2.54</f>
         <v>26.377952755905511</v>
       </c>
     </row>
     <row r="44" spans="8:11" ht="16.5" customHeight="1">
-      <c r="H44" s="94"/>
-      <c r="I44" s="42" t="s">
-        <v>178</v>
-      </c>
-      <c r="J44" s="55">
+      <c r="H44" s="76"/>
+      <c r="I44" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J44" s="50">
         <f>J40+27</f>
         <v>67</v>
       </c>
-      <c r="K44" s="55">
+      <c r="K44" s="50">
         <f>J44/2.54</f>
         <v>26.377952755905511</v>
       </c>
     </row>
     <row r="45" spans="8:11">
-      <c r="H45" s="94"/>
-      <c r="I45" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="J45" s="55">
+      <c r="H45" s="76"/>
+      <c r="I45" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="J45" s="50">
         <f>J41+20</f>
         <v>45</v>
       </c>
-      <c r="K45" s="55">
+      <c r="K45" s="50">
         <f>J45/2.54</f>
         <v>17.716535433070867</v>
       </c>
     </row>
     <row r="47" spans="8:11">
-      <c r="H47" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="I47" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="J47" s="55">
+      <c r="H47" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="I47" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="J47" s="50">
         <f>2.54*K47</f>
         <v>39.92</v>
       </c>
-      <c r="K47" s="55">
+      <c r="K47" s="50">
         <f>K45-2</f>
         <v>15.716535433070867</v>
       </c>
@@ -3961,8 +3956,8 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="46" spans="1:1">
-      <c r="A46" s="46" t="s">
-        <v>153</v>
+      <c r="A46" s="41" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3986,8 +3981,8 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="54" spans="1:1">
-      <c r="A54" s="46" t="s">
-        <v>155</v>
+      <c r="A54" s="41" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4011,8 +4006,8 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="55" spans="1:1">
-      <c r="A55" s="46" t="s">
-        <v>154</v>
+      <c r="A55" s="41" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4036,8 +4031,8 @@
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="46" t="s">
-        <v>156</v>
+      <c r="A1" s="41" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
src and belt clip added
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\Mostly-Printed-CNC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\03.Mostly-Printed-CNC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="250">
   <si>
     <t>QTY</t>
   </si>
@@ -834,22 +834,38 @@
   <si>
     <t>Power (12V HC) - high current</t>
   </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="166" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="169" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
   </numFmts>
   <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -878,14 +894,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -906,7 +922,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -915,7 +931,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -924,7 +940,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -962,14 +978,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -990,7 +1006,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -998,14 +1014,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1013,7 +1029,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1021,7 +1037,7 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1030,7 +1046,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1038,7 +1054,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1250,7 +1266,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1317,19 +1333,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1344,7 +1360,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -1377,310 +1393,313 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2192,7 +2211,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2456,20 +2475,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.875" customWidth="1"/>
+    <col min="2" max="2" width="38.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2507,31 +2526,31 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="73">
+      <c r="C4" s="63">
         <v>4</v>
       </c>
-      <c r="D4" s="75">
+      <c r="D4" s="65">
         <v>0.4</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="63">
         <v>59.3</v>
       </c>
-      <c r="G4" s="73">
+      <c r="G4" s="63">
         <v>234.5</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="67" t="s">
         <v>148</v>
       </c>
-      <c r="I4" s="78" t="s">
+      <c r="I4" s="68" t="s">
         <v>137</v>
       </c>
       <c r="J4" s="38">
@@ -2539,29 +2558,29 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="108"/>
-      <c r="B5" s="74" t="s">
+      <c r="A5" s="119"/>
+      <c r="B5" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="63">
         <v>4</v>
       </c>
-      <c r="D5" s="75">
+      <c r="D5" s="65">
         <v>0.7</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="63">
         <v>17.5</v>
       </c>
-      <c r="G5" s="73">
+      <c r="G5" s="63">
         <v>70.099999999999994</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="67" t="s">
         <v>147</v>
       </c>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="68" t="s">
         <v>137</v>
       </c>
       <c r="J5" s="38">
@@ -2569,31 +2588,31 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="120" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="88">
+      <c r="C6" s="76">
         <v>4</v>
       </c>
-      <c r="D6" s="89">
+      <c r="D6" s="77">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E6" s="90" t="s">
+      <c r="E6" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="88">
+      <c r="F6" s="76">
         <v>89.6</v>
       </c>
-      <c r="G6" s="88">
+      <c r="G6" s="76">
         <v>363</v>
       </c>
-      <c r="H6" s="96" t="s">
+      <c r="H6" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="I6" s="92" t="s">
+      <c r="I6" s="80" t="s">
         <v>139</v>
       </c>
       <c r="J6" s="38">
@@ -2601,29 +2620,29 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="86"/>
-      <c r="B7" s="87" t="s">
+      <c r="A7" s="121"/>
+      <c r="B7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="88">
+      <c r="C7" s="76">
         <v>4</v>
       </c>
-      <c r="D7" s="89">
+      <c r="D7" s="77">
         <v>0.7</v>
       </c>
-      <c r="E7" s="90" t="s">
+      <c r="E7" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="88">
+      <c r="F7" s="76">
         <v>20.8</v>
       </c>
-      <c r="G7" s="88">
+      <c r="G7" s="76">
         <v>83</v>
       </c>
-      <c r="H7" s="96" t="s">
+      <c r="H7" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="92" t="s">
+      <c r="I7" s="80" t="s">
         <v>138</v>
       </c>
       <c r="J7" s="38">
@@ -2631,29 +2650,29 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="87" t="s">
+      <c r="A8" s="122"/>
+      <c r="B8" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="76">
         <v>4</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="77">
         <v>0.7</v>
       </c>
-      <c r="E8" s="90" t="s">
+      <c r="E8" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="76">
         <v>30.8</v>
       </c>
-      <c r="G8" s="88">
+      <c r="G8" s="76">
         <v>123.5</v>
       </c>
-      <c r="H8" s="96" t="s">
+      <c r="H8" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="92" t="s">
         <v>140</v>
       </c>
       <c r="J8" s="38">
@@ -2661,31 +2680,31 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="123" t="s">
         <v>195</v>
       </c>
-      <c r="B9" s="74" t="s">
+      <c r="B9" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="63">
         <v>2</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="65">
         <v>0.75</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="63">
         <v>66</v>
       </c>
-      <c r="G9" s="73">
+      <c r="G9" s="63">
         <v>132</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="I9" s="78" t="s">
+      <c r="I9" s="68" t="s">
         <v>165</v>
       </c>
       <c r="J9" s="38">
@@ -2693,29 +2712,29 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="110"/>
-      <c r="B10" s="74" t="s">
+      <c r="A10" s="124"/>
+      <c r="B10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="63">
         <v>2</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="65">
         <v>0.7</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="63">
         <v>110.6</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="78" t="s">
+      <c r="I10" s="68" t="s">
         <v>119</v>
       </c>
       <c r="J10" s="38">
@@ -2723,350 +2742,376 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="110"/>
-      <c r="B11" s="74" t="s">
+      <c r="A11" s="124"/>
+      <c r="B11" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="73">
+      <c r="C11" s="63">
         <v>2</v>
       </c>
-      <c r="D11" s="75">
+      <c r="D11" s="65">
         <v>0.7</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="E11" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="73">
+      <c r="G11" s="63">
         <v>105</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="H11" s="67" t="s">
         <v>144</v>
       </c>
-      <c r="I11" s="78"/>
+      <c r="I11" s="68" t="s">
+        <v>246</v>
+      </c>
+      <c r="J11" s="38">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="111"/>
-      <c r="B12" s="74" t="s">
+      <c r="A12" s="125"/>
+      <c r="B12" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="73">
+      <c r="C12" s="63">
         <v>1</v>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="65">
         <v>0.7</v>
       </c>
-      <c r="E12" s="76" t="s">
+      <c r="E12" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="73">
+      <c r="G12" s="63">
         <v>12</v>
       </c>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="67" t="s">
         <v>152</v>
       </c>
-      <c r="I12" s="78"/>
+      <c r="I12" s="68" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="120" t="s">
         <v>196</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="88">
+      <c r="C13" s="76">
         <v>2</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="77">
         <v>0.5</v>
       </c>
-      <c r="E13" s="90" t="s">
+      <c r="E13" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="82" t="s">
         <v>158</v>
       </c>
-      <c r="I13" s="92"/>
+      <c r="I13" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="J13" s="38">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="86"/>
-      <c r="B14" s="87" t="s">
+      <c r="A14" s="121"/>
+      <c r="B14" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="88">
+      <c r="C14" s="76">
         <v>1</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="77">
         <v>0.6</v>
       </c>
-      <c r="E14" s="90" t="s">
+      <c r="E14" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="88" t="s">
+      <c r="F14" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="88">
+      <c r="G14" s="76">
         <v>39</v>
       </c>
-      <c r="H14" s="96" t="s">
+      <c r="H14" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="I14" s="92"/>
+      <c r="I14" s="80" t="s">
+        <v>246</v>
+      </c>
+      <c r="J14" s="38">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="86"/>
-      <c r="B15" s="87" t="s">
+      <c r="A15" s="121"/>
+      <c r="B15" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="88">
+      <c r="C15" s="76">
         <v>1</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="77">
         <v>0.5</v>
       </c>
-      <c r="E15" s="90" t="s">
+      <c r="E15" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="88" t="s">
+      <c r="F15" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="88" t="s">
+      <c r="G15" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="96" t="s">
+      <c r="H15" s="83" t="s">
         <v>161</v>
       </c>
-      <c r="I15" s="92"/>
+      <c r="I15" s="80" t="s">
+        <v>248</v>
+      </c>
+      <c r="J15" s="38">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="86"/>
-      <c r="B16" s="97" t="s">
+      <c r="A16" s="121"/>
+      <c r="B16" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="98">
+      <c r="C16" s="85">
         <v>1</v>
       </c>
-      <c r="D16" s="99">
+      <c r="D16" s="86">
         <v>0.7</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="98" t="s">
+      <c r="F16" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="85">
         <v>5.7</v>
       </c>
-      <c r="H16" s="101" t="s">
+      <c r="H16" s="88" t="s">
         <v>157</v>
       </c>
-      <c r="I16" s="102"/>
+      <c r="I16" s="89"/>
     </row>
     <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="94"/>
-      <c r="B17" s="87" t="s">
+      <c r="A17" s="122"/>
+      <c r="B17" s="75" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="88">
+      <c r="C17" s="76">
         <v>1</v>
       </c>
-      <c r="D17" s="89"/>
-      <c r="E17" s="90" t="s">
+      <c r="D17" s="77"/>
+      <c r="E17" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="103" t="s">
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="90" t="s">
         <v>156</v>
       </c>
-      <c r="I17" s="104"/>
+      <c r="I17" s="91"/>
     </row>
     <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="123" t="s">
         <v>198</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="73">
+      <c r="C18" s="63">
         <v>4</v>
       </c>
-      <c r="D18" s="75">
+      <c r="D18" s="65">
         <v>0.6</v>
       </c>
-      <c r="E18" s="76" t="s">
+      <c r="E18" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="73" t="s">
+      <c r="F18" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="73">
+      <c r="G18" s="63">
         <v>148.1</v>
       </c>
-      <c r="H18" s="77" t="s">
+      <c r="H18" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="I18" s="78"/>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="111"/>
-      <c r="B19" s="74" t="s">
+      <c r="A19" s="125"/>
+      <c r="B19" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="C19" s="73">
+      <c r="C19" s="63">
         <v>4</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="65">
         <v>0.6</v>
       </c>
-      <c r="E19" s="76" t="s">
+      <c r="E19" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="73">
+      <c r="F19" s="63">
         <v>31.8</v>
       </c>
-      <c r="G19" s="73">
+      <c r="G19" s="63">
         <v>127.1</v>
       </c>
-      <c r="H19" s="77" t="s">
+      <c r="H19" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="I19" s="78"/>
+      <c r="I19" s="68"/>
     </row>
     <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="120" t="s">
         <v>205</v>
       </c>
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="81">
+      <c r="C20" s="70">
         <v>2</v>
       </c>
-      <c r="D20" s="82">
+      <c r="D20" s="71">
         <v>0.7</v>
       </c>
-      <c r="E20" s="83" t="s">
+      <c r="E20" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="81" t="s">
+      <c r="G20" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="84" t="s">
+      <c r="H20" s="73" t="s">
         <v>164</v>
       </c>
-      <c r="I20" s="85"/>
+      <c r="I20" s="74"/>
       <c r="J20" s="30"/>
       <c r="K20" s="31"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="86"/>
-      <c r="B21" s="87" t="s">
+      <c r="A21" s="121"/>
+      <c r="B21" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="88">
+      <c r="C21" s="76">
         <v>1</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="77">
         <v>0.7</v>
       </c>
-      <c r="E21" s="90" t="s">
+      <c r="E21" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="91" t="s">
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="79" t="s">
         <v>143</v>
       </c>
-      <c r="I21" s="92"/>
-      <c r="J21" s="30"/>
+      <c r="I21" s="80" t="s">
+        <v>249</v>
+      </c>
+      <c r="J21" s="142">
+        <v>0.4</v>
+      </c>
       <c r="K21" s="31"/>
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="30">
-      <c r="A22" s="86"/>
-      <c r="B22" s="87" t="s">
+    <row r="22" spans="1:12" ht="33">
+      <c r="A22" s="121"/>
+      <c r="B22" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="88">
+      <c r="C22" s="76">
         <v>1</v>
       </c>
-      <c r="D22" s="89">
+      <c r="D22" s="77">
         <v>0.7</v>
       </c>
-      <c r="E22" s="90" t="s">
+      <c r="E22" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="93" t="s">
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="81" t="s">
         <v>159</v>
       </c>
-      <c r="I22" s="92"/>
+      <c r="I22" s="80"/>
       <c r="J22" s="30"/>
       <c r="K22" s="31"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1">
-      <c r="A23" s="86"/>
-      <c r="B23" s="87" t="s">
+      <c r="A23" s="121"/>
+      <c r="B23" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="C23" s="88">
+      <c r="C23" s="76">
         <v>1</v>
       </c>
-      <c r="D23" s="89">
+      <c r="D23" s="77">
         <v>0.7</v>
       </c>
-      <c r="E23" s="90" t="s">
+      <c r="E23" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="93" t="s">
+      <c r="F23" s="76"/>
+      <c r="G23" s="76"/>
+      <c r="H23" s="81" t="s">
         <v>197</v>
       </c>
-      <c r="I23" s="92"/>
+      <c r="I23" s="80"/>
       <c r="J23" s="30"/>
       <c r="K23" s="31"/>
       <c r="L23" s="6"/>
     </row>
-    <row r="24" spans="1:12" ht="30">
-      <c r="A24" s="94"/>
-      <c r="B24" s="87" t="s">
+    <row r="24" spans="1:12" ht="33">
+      <c r="A24" s="122"/>
+      <c r="B24" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="C24" s="88">
+      <c r="C24" s="76">
         <v>1</v>
       </c>
-      <c r="D24" s="89">
+      <c r="D24" s="77">
         <v>0.7</v>
       </c>
-      <c r="E24" s="90" t="s">
+      <c r="E24" s="78" t="s">
         <v>141</v>
       </c>
-      <c r="F24" s="88"/>
-      <c r="G24" s="88"/>
-      <c r="H24" s="93" t="s">
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="I24" s="92"/>
+      <c r="I24" s="80"/>
     </row>
     <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="1"/>
@@ -3085,10 +3130,10 @@
       <c r="C26" s="17">
         <v>1</v>
       </c>
-      <c r="D26" s="127">
+      <c r="D26" s="103">
         <v>0.7</v>
       </c>
-      <c r="E26" s="90" t="s">
+      <c r="E26" s="78" t="s">
         <v>141</v>
       </c>
       <c r="F26" s="17"/>
@@ -3102,12 +3147,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A20:A24"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A20:A24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -3147,11 +3192,11 @@
       <selection activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
@@ -3175,7 +3220,7 @@
       <c r="A2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="44" t="s">
         <v>168</v>
       </c>
       <c r="C2" s="25" t="s">
@@ -3184,7 +3229,7 @@
       <c r="D2" s="22">
         <v>8500</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="42" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3192,7 +3237,7 @@
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>169</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -3209,7 +3254,7 @@
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="44" t="s">
         <v>170</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -3227,7 +3272,7 @@
       <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="44" t="s">
         <v>171</v>
       </c>
       <c r="C5" s="25">
@@ -3244,7 +3289,7 @@
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="45" t="s">
         <v>172</v>
       </c>
       <c r="C6" s="25">
@@ -3262,7 +3307,7 @@
       <c r="A7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="44" t="s">
         <v>173</v>
       </c>
       <c r="C7" s="25" t="s">
@@ -3280,7 +3325,7 @@
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="44" t="s">
         <v>174</v>
       </c>
       <c r="C8" s="25">
@@ -3298,7 +3343,7 @@
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="45" t="s">
         <v>177</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -3315,7 +3360,7 @@
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="44" t="s">
         <v>175</v>
       </c>
       <c r="C10" s="10">
@@ -3333,7 +3378,7 @@
       <c r="A11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="44" t="s">
         <v>176</v>
       </c>
       <c r="C11" s="10">
@@ -3350,7 +3395,7 @@
       <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="46"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="10">
         <v>1</v>
       </c>
@@ -3361,7 +3406,7 @@
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="10"/>
-      <c r="B13" s="46"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="10"/>
       <c r="D13" s="23"/>
       <c r="E13" s="33"/>
@@ -3370,7 +3415,7 @@
       <c r="A14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="46"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="10" t="s">
         <v>35</v>
       </c>
@@ -3383,7 +3428,7 @@
       <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="46"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="10">
         <v>4</v>
       </c>
@@ -3396,12 +3441,12 @@
       <c r="A16" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="24"/>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="43" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3507,7 +3552,8 @@
     <hyperlink ref="B24" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3519,22 +3565,22 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.375" customWidth="1"/>
+    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1">
@@ -3562,10 +3608,10 @@
       <c r="H1" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="65"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="62" t="s">
         <v>190</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -3583,13 +3629,13 @@
       <c r="F2" s="22">
         <v>1500</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="42" t="s">
         <v>119</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="64"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="35"/>
       <c r="K2" s="29"/>
       <c r="L2" s="29" t="s">
@@ -3600,32 +3646,32 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="126" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="133" t="s">
         <v>183</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F3" s="22">
         <v>1500</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="42" t="s">
+      <c r="I3" s="59"/>
+      <c r="J3" s="131" t="s">
         <v>133</v>
       </c>
       <c r="K3" s="29" t="s">
@@ -3640,14 +3686,14 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="69"/>
+      <c r="A4" s="127"/>
       <c r="B4" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="134"/>
       <c r="E4" s="10" t="s">
         <v>58</v>
       </c>
@@ -3660,8 +3706,8 @@
       <c r="H4" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="43"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="132"/>
       <c r="K4" s="29" t="s">
         <v>126</v>
       </c>
@@ -3674,14 +3720,14 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="69"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="134"/>
       <c r="E5" s="10" t="s">
         <v>61</v>
       </c>
@@ -3694,8 +3740,8 @@
       <c r="H5" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="I5" s="64"/>
-      <c r="J5" s="43"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="29" t="s">
         <v>127</v>
       </c>
@@ -3708,14 +3754,14 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="69"/>
+      <c r="A6" s="127"/>
       <c r="B6" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="50"/>
+      <c r="D6" s="134"/>
       <c r="E6" s="10" t="s">
         <v>61</v>
       </c>
@@ -3728,21 +3774,21 @@
       <c r="H6" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="64"/>
+      <c r="I6" s="59"/>
       <c r="J6" s="36"/>
       <c r="K6" s="36"/>
       <c r="L6" s="36"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="70"/>
+      <c r="A7" s="128"/>
       <c r="B7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="135"/>
       <c r="E7" s="11">
         <v>28</v>
       </c>
@@ -3750,14 +3796,14 @@
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="42" t="s">
+      <c r="I7" s="59"/>
+      <c r="J7" s="131" t="s">
         <v>134</v>
       </c>
       <c r="K7" s="29" t="s">
@@ -3773,32 +3819,32 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="129" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="51">
         <v>1500</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="H8" s="57" t="s">
+      <c r="H8" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="42"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="131"/>
       <c r="K8" s="29" t="s">
         <v>131</v>
       </c>
@@ -3812,30 +3858,30 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="72"/>
-      <c r="B9" s="58" t="s">
+      <c r="A9" s="130"/>
+      <c r="B9" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="60">
+      <c r="F9" s="55">
         <v>1500</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="42"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="131"/>
       <c r="K9" s="29" t="s">
         <v>132</v>
       </c>
@@ -3849,42 +3895,42 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="133" t="s">
         <v>180</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="48" t="s">
         <v>69</v>
       </c>
       <c r="F10" s="22">
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="64"/>
+      <c r="I10" s="59"/>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="69"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="134"/>
       <c r="E11" s="10" t="s">
         <v>71</v>
       </c>
@@ -3897,7 +3943,7 @@
       <c r="H11" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="I11" s="64"/>
+      <c r="I11" s="59"/>
       <c r="J11" s="29" t="s">
         <v>135</v>
       </c>
@@ -3914,64 +3960,64 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="70"/>
+      <c r="A12" s="128"/>
       <c r="B12" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="51"/>
+      <c r="D12" s="135"/>
       <c r="E12" s="11">
         <v>36</v>
       </c>
-      <c r="F12" s="49">
+      <c r="F12" s="47">
         <v>1500</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="64"/>
+      <c r="I12" s="59"/>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="126" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="133" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="48" t="s">
         <v>77</v>
       </c>
       <c r="F13" s="22">
         <v>1500</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="I13" s="64"/>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="69"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="50"/>
+      <c r="D14" s="134"/>
       <c r="E14" s="10">
         <v>34</v>
       </c>
@@ -3984,53 +4030,53 @@
       <c r="H14" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="I14" s="64"/>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="70"/>
+      <c r="A15" s="128"/>
       <c r="B15" s="11" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="135"/>
       <c r="E15" s="11" t="s">
         <v>81</v>
       </c>
       <c r="F15" s="24">
         <v>1500</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="64"/>
+      <c r="I15" s="59"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="126" t="s">
         <v>189</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="52" t="s">
+      <c r="D16" s="61"/>
+      <c r="E16" s="48" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="22"/>
-      <c r="G16" s="44"/>
+      <c r="G16" s="42"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="64"/>
+      <c r="I16" s="59"/>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="70"/>
+      <c r="A17" s="128"/>
       <c r="B17" s="11" t="s">
         <v>75</v>
       </c>
@@ -4042,9 +4088,9 @@
         <v>23</v>
       </c>
       <c r="F17" s="24"/>
-      <c r="G17" s="45"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="64"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="1:9">
       <c r="B18" s="34" t="s">
@@ -4054,13 +4100,13 @@
         <f>SUM(F2:F15)</f>
         <v>25500</v>
       </c>
-      <c r="I18" s="63"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9">
       <c r="B19" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="62"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="27" spans="1:9">
       <c r="E27" s="6"/>
@@ -4069,16 +4115,16 @@
     <row r="44" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4098,7 +4144,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="46" spans="1:1">
       <c r="A46" s="32" t="s">
@@ -4123,7 +4169,7 @@
       <selection activeCell="AJ38" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="54" spans="1:1">
       <c r="A54" s="32" t="s">
@@ -4148,7 +4194,7 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="55" spans="1:1">
       <c r="A55" s="32" t="s">
@@ -4173,7 +4219,7 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="32" t="s">
@@ -4199,226 +4245,226 @@
       <selection activeCell="H5" sqref="H5:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="19" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="37.625" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="19" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75">
-      <c r="A1" s="126" t="s">
+    <row r="1" spans="1:19" ht="20.25">
+      <c r="A1" s="102" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="102" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="126" t="s">
+      <c r="C1" s="102" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="102" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="102" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="136" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="96" t="s">
         <v>206</v>
       </c>
       <c r="C2" s="41">
         <v>4</v>
       </c>
-      <c r="D2" s="116">
+      <c r="D2" s="138">
         <v>4</v>
       </c>
-      <c r="E2" s="116">
+      <c r="E2" s="138">
         <v>6</v>
       </c>
-      <c r="H2" s="128">
+      <c r="H2" s="104">
         <v>1</v>
       </c>
-      <c r="I2" s="128">
+      <c r="I2" s="104">
         <v>2</v>
       </c>
-      <c r="J2" s="128">
+      <c r="J2" s="104">
         <v>3</v>
       </c>
-      <c r="K2" s="128">
+      <c r="K2" s="104">
         <v>4</v>
       </c>
-      <c r="L2" s="128">
+      <c r="L2" s="104">
         <v>5</v>
       </c>
-      <c r="M2" s="128">
+      <c r="M2" s="104">
         <v>6</v>
       </c>
-      <c r="N2" s="122">
+      <c r="N2" s="100">
         <v>7</v>
       </c>
-      <c r="O2" s="122">
+      <c r="O2" s="100">
         <v>8</v>
       </c>
-      <c r="P2" s="122">
+      <c r="P2" s="100">
         <v>9</v>
       </c>
-      <c r="Q2" s="122">
+      <c r="Q2" s="100">
         <v>10</v>
       </c>
-      <c r="R2" s="122">
+      <c r="R2" s="100">
         <v>11</v>
       </c>
-      <c r="S2" s="122">
+      <c r="S2" s="100">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="113"/>
-      <c r="B3" s="118" t="s">
+      <c r="A3" s="137"/>
+      <c r="B3" s="96" t="s">
         <v>207</v>
       </c>
       <c r="C3" s="41">
         <v>2</v>
       </c>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="H3" s="128" t="s">
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="H3" s="104" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="128" t="s">
+      <c r="I3" s="104" t="s">
         <v>220</v>
       </c>
-      <c r="J3" s="128" t="s">
+      <c r="J3" s="104" t="s">
         <v>221</v>
       </c>
-      <c r="K3" s="128" t="s">
+      <c r="K3" s="104" t="s">
         <v>222</v>
       </c>
-      <c r="L3" s="128" t="s">
+      <c r="L3" s="104" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="128" t="s">
+      <c r="M3" s="104" t="s">
         <v>223</v>
       </c>
-      <c r="N3" s="122" t="s">
+      <c r="N3" s="100" t="s">
         <v>210</v>
       </c>
-      <c r="O3" s="122"/>
-      <c r="P3" s="138" t="s">
+      <c r="O3" s="100"/>
+      <c r="P3" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="Q3" s="139" t="s">
+      <c r="Q3" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="R3" s="140" t="s">
+      <c r="R3" s="116" t="s">
         <v>241</v>
       </c>
-      <c r="S3" s="141" t="s">
+      <c r="S3" s="117" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="113"/>
-      <c r="B4" s="136" t="s">
+      <c r="A4" s="137"/>
+      <c r="B4" s="112" t="s">
         <v>242</v>
       </c>
       <c r="C4" s="41">
         <v>1</v>
       </c>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="132"/>
-      <c r="N4" s="132"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="134"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="132"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="H4" s="108"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="108"/>
+      <c r="K4" s="108"/>
+      <c r="L4" s="108"/>
+      <c r="M4" s="108"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="110"/>
+      <c r="R4" s="111"/>
+      <c r="S4" s="108"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="113"/>
-      <c r="B5" s="137" t="s">
+      <c r="A5" s="137"/>
+      <c r="B5" s="113" t="s">
         <v>243</v>
       </c>
       <c r="C5" s="41">
         <v>1</v>
       </c>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
+      <c r="D5" s="139"/>
+      <c r="E5" s="139"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="113"/>
-      <c r="B6" s="130" t="s">
+      <c r="A6" s="137"/>
+      <c r="B6" s="106" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="115">
+      <c r="C6" s="94">
         <v>1</v>
       </c>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="139"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="113"/>
-      <c r="B7" s="119" t="s">
+      <c r="A7" s="137"/>
+      <c r="B7" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="C7" s="115">
+      <c r="C7" s="94">
         <v>1</v>
       </c>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="136" t="s">
         <v>209</v>
       </c>
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="95">
         <v>1</v>
       </c>
-      <c r="D8" s="116">
+      <c r="D8" s="138">
         <v>2</v>
       </c>
-      <c r="E8" s="116">
+      <c r="E8" s="138">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="113"/>
-      <c r="B9" s="120" t="s">
+      <c r="A9" s="137"/>
+      <c r="B9" s="98" t="s">
         <v>218</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="95">
         <v>1</v>
       </c>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
       <c r="H9" t="s">
         <v>227</v>
       </c>
       <c r="J9" t="s">
         <v>226</v>
       </c>
-      <c r="K9" s="129">
+      <c r="K9" s="105">
         <v>390</v>
       </c>
       <c r="L9">
         <v>2</v>
       </c>
-      <c r="M9" s="129">
+      <c r="M9" s="105">
         <f t="shared" ref="M9:M14" si="0">K9*L9</f>
         <v>780</v>
       </c>
@@ -4427,17 +4473,17 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="114"/>
-      <c r="B10" s="121" t="s">
+      <c r="A10" s="141"/>
+      <c r="B10" s="99" t="s">
         <v>210</v>
       </c>
       <c r="C10" s="37">
         <v>1</v>
       </c>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
-      <c r="K10" s="129"/>
-      <c r="M10" s="129"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="140"/>
+      <c r="K10" s="105"/>
+      <c r="M10" s="105"/>
       <c r="N10" s="32"/>
     </row>
     <row r="11" spans="1:19">
@@ -4447,13 +4493,13 @@
       <c r="J11" t="s">
         <v>229</v>
       </c>
-      <c r="K11" s="129">
+      <c r="K11" s="105">
         <v>500</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" s="129">
+      <c r="M11" s="105">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
@@ -4462,19 +4508,19 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="100" t="s">
         <v>211</v>
       </c>
-      <c r="B13" s="123" t="s">
+      <c r="B13" s="101" t="s">
         <v>212</v>
       </c>
-      <c r="C13" s="122">
+      <c r="C13" s="100">
         <v>2</v>
       </c>
-      <c r="D13" s="122">
+      <c r="D13" s="100">
         <v>0</v>
       </c>
-      <c r="E13" s="122">
+      <c r="E13" s="100">
         <v>2</v>
       </c>
       <c r="H13" t="s">
@@ -4483,13 +4529,13 @@
       <c r="J13" t="s">
         <v>232</v>
       </c>
-      <c r="K13" s="129">
+      <c r="K13" s="105">
         <v>210</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="M13" s="129">
+      <c r="M13" s="105">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
@@ -4504,13 +4550,13 @@
       <c r="J14" t="s">
         <v>231</v>
       </c>
-      <c r="K14" s="129">
+      <c r="K14" s="105">
         <v>510</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
-      <c r="M14" s="129">
+      <c r="M14" s="105">
         <f t="shared" si="0"/>
         <v>510</v>
       </c>
@@ -4522,13 +4568,13 @@
       <c r="H15" t="s">
         <v>238</v>
       </c>
-      <c r="K15" s="129">
+      <c r="K15" s="105">
         <v>50</v>
       </c>
       <c r="L15">
         <v>20</v>
       </c>
-      <c r="M15" s="129">
+      <c r="M15" s="105">
         <f>K15*L15</f>
         <v>1000</v>
       </c>
@@ -4545,6 +4591,7 @@
     <mergeCell ref="E2:E7"/>
     <mergeCell ref="E8:E10"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N9" r:id="rId1"/>
     <hyperlink ref="N11" r:id="rId2"/>

</xml_diff>

<commit_message>
motor step and knob direction changed
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\03.Mostly-Printed-CNC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\Mostly-Printed-CNC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="259">
   <si>
     <t>QTY</t>
   </si>
@@ -156,34 +156,10 @@
     <t>Spindle Options</t>
   </si>
   <si>
-    <t>Best option</t>
-  </si>
-  <si>
     <t>Dewalt 660 (Beast!)</t>
   </si>
   <si>
     <t>http://amzn.to/1VyeDY6</t>
-  </si>
-  <si>
-    <t>Second Choice</t>
-  </si>
-  <si>
-    <t>Flex shaft 1/4 HP</t>
-  </si>
-  <si>
-    <t>http://amzn.to/1CxOqmt</t>
-  </si>
-  <si>
-    <t>44T for the collets</t>
-  </si>
-  <si>
-    <t>http://amzn.to/1L04pwh</t>
-  </si>
-  <si>
-    <t>White lithium</t>
-  </si>
-  <si>
-    <t>http://amzn.to/1O3LtLq</t>
   </si>
   <si>
     <t>Imperial</t>
@@ -855,16 +831,56 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>ETC</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> riemenhalter.stl</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>V</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>End stops</t>
+  </si>
+  <si>
+    <t>IE25mm-A-endstops_XY.stl
+IE25mm-B-endstops_Z.stl</t>
+  </si>
+  <si>
+    <t>riemenhalter.stl</t>
+  </si>
+  <si>
+    <t>RepRapDiscount Full Graphic Smart Controller</t>
+  </si>
+  <si>
+    <t>mods_for_display_case_button.stl
+mods_for_display_case_front.stl
+mods_for_display_case_back.stl</t>
+  </si>
+  <si>
+    <t>3D printer extruder</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/12-24V-Fan-3D-Printer-head-Makerbot-3D-Printer-single-exturder-MK8-Extruder-Free-Shipping/1987122502.html</t>
+  </si>
+  <si>
+    <t>3D Printer Options</t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/500mw-405NM-focusing-blue-purple-laser-module-laser-engraving-TTL-module-500mw-laser-tube-Laser-module/32562052620.html</t>
+  </si>
+  <si>
+    <t>Laser Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500mw 405NM focusing blue purple laser module laser engraving TTL module </t>
+  </si>
+  <si>
+    <t>http://www.aliexpress.com/item/1pc-Gcc-Signpal-Vinyl-Cutter-Blade-Holder-5-pcs-45-5-pcs-60-Degree-Roland-Liyu/32336073909.html</t>
+  </si>
+  <si>
+    <t>Gcc Sign pal Vinyl Cutter Blade Holder + 5 pcs 45 + 5 pcs 60 Degree</t>
+  </si>
+  <si>
+    <t>Roland Drag Knife Options</t>
+  </si>
+  <si>
+    <t>or Dremel 300</t>
   </si>
 </sst>
 </file>
@@ -872,16 +888,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="179" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="167" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
   </numFmts>
   <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -910,14 +926,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -938,7 +954,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -947,7 +963,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -956,7 +972,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -994,14 +1010,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1022,7 +1038,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1030,14 +1046,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1045,7 +1061,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1053,7 +1069,7 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1062,7 +1078,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1070,7 +1086,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1129,7 +1145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1183,15 +1199,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1282,23 +1289,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -1307,61 +1308,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1373,7 +1353,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -1388,7 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1412,16 +1392,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,10 +1410,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1442,10 +1422,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1457,13 +1437,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1532,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1568,7 +1548,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1649,51 +1629,81 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1723,8 +1733,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1748,16 +1758,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>17600</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>18093</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>75243</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1774,7 +1784,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="6496050"/>
+          <a:off x="14154150" y="0"/>
           <a:ext cx="11600000" cy="7657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2236,7 +2246,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2498,700 +2508,748 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="44.875" customWidth="1"/>
-    <col min="2" max="2" width="38.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A4" s="123" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="53">
+        <v>4</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="53">
+        <v>59.3</v>
+      </c>
+      <c r="G4" s="53">
+        <v>234.5</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A5" s="124"/>
+      <c r="B5" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="53">
+        <v>4</v>
+      </c>
+      <c r="D5" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="53">
+        <v>17.5</v>
+      </c>
+      <c r="G5" s="53">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A6" s="125" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="60">
+        <v>4</v>
+      </c>
+      <c r="D6" s="61">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="60">
+        <v>89.6</v>
+      </c>
+      <c r="G6" s="60">
+        <v>363</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A7" s="126"/>
+      <c r="B7" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="60">
+        <v>4</v>
+      </c>
+      <c r="D7" s="61">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="60">
+        <v>20.8</v>
+      </c>
+      <c r="G7" s="60">
+        <v>83</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="63" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A8" s="127"/>
+      <c r="B8" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="60">
+        <v>4</v>
+      </c>
+      <c r="D8" s="61">
+        <v>0.7</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="60">
+        <v>30.8</v>
+      </c>
+      <c r="G8" s="60">
+        <v>123.5</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="28">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A9" s="120" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="53">
+        <v>2</v>
+      </c>
+      <c r="D9" s="55">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="53">
+        <v>66</v>
+      </c>
+      <c r="G9" s="53">
+        <v>132</v>
+      </c>
+      <c r="H9" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>157</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A10" s="121"/>
+      <c r="B10" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="53">
+        <v>2</v>
+      </c>
+      <c r="D10" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E10" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="53">
+        <v>110.6</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A11" s="121"/>
+      <c r="B11" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="53">
+        <v>2</v>
+      </c>
+      <c r="D11" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="53" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="G11" s="53">
+        <v>105</v>
+      </c>
+      <c r="H11" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A12" s="122"/>
+      <c r="B12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="53">
+        <v>1</v>
+      </c>
+      <c r="D12" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="53">
+        <v>12</v>
+      </c>
+      <c r="H12" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A13" s="125" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="60">
+        <v>2</v>
+      </c>
+      <c r="D13" s="61">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="J13" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A14" s="126"/>
+      <c r="B14" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="60">
+        <v>1</v>
+      </c>
+      <c r="D14" s="61">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" s="60">
+        <v>39</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="J14" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A15" s="126"/>
+      <c r="B15" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="60">
+        <v>1</v>
+      </c>
+      <c r="D15" s="61">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="65" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="J15" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.5" customHeight="1">
+      <c r="A16" s="126"/>
+      <c r="B16" s="66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="67">
+        <v>1</v>
+      </c>
+      <c r="D16" s="68">
+        <v>0.7</v>
+      </c>
+      <c r="E16" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="67">
+        <v>5.7</v>
+      </c>
+      <c r="H16" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="I16" s="71"/>
+    </row>
+    <row r="17" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A17" s="127"/>
+      <c r="B17" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="60">
+        <v>1</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17" s="73" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A18" s="120" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="53">
+        <v>4</v>
+      </c>
+      <c r="D18" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="53">
+        <v>148.1</v>
+      </c>
+      <c r="H18" s="57" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" s="28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A19" s="122"/>
+      <c r="B19" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="53">
+        <v>4</v>
+      </c>
+      <c r="D19" s="55">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="53">
+        <v>31.8</v>
+      </c>
+      <c r="G19" s="53">
+        <v>127.1</v>
+      </c>
+      <c r="H19" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="I19" s="58"/>
+    </row>
+    <row r="20" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A20" s="128" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="102" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="102">
+        <v>8</v>
+      </c>
+      <c r="D20" s="103">
+        <v>0.4</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="102"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="65" t="s">
+        <v>246</v>
+      </c>
+      <c r="I20" s="63" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A21" s="129"/>
+      <c r="B21" s="102" t="s">
+        <v>244</v>
+      </c>
+      <c r="C21" s="102">
+        <v>1</v>
+      </c>
+      <c r="D21" s="103">
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="102"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="114" t="s">
+        <v>245</v>
+      </c>
+      <c r="I21" s="63"/>
+    </row>
+    <row r="22" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A22" s="130"/>
+      <c r="B22" s="102" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="102">
+        <v>1</v>
+      </c>
+      <c r="D22" s="103">
+        <v>0.4</v>
+      </c>
+      <c r="E22" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="102"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="I22" s="63"/>
+    </row>
+    <row r="23" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A23" s="120" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="104" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="105">
+        <v>2</v>
+      </c>
+      <c r="D23" s="106">
+        <v>0.7</v>
+      </c>
+      <c r="E23" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="108" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" s="109"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A24" s="121"/>
+      <c r="B24" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="53">
+        <v>1</v>
+      </c>
+      <c r="D24" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="110" t="s">
+        <v>135</v>
+      </c>
+      <c r="I24" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="J24" s="99">
+        <v>0.4</v>
+      </c>
+      <c r="K24" s="21"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A25" s="121"/>
+      <c r="B25" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C25" s="53">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="125" t="s">
-        <v>193</v>
-      </c>
-      <c r="B4" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="62">
-        <v>4</v>
-      </c>
-      <c r="D4" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="62">
-        <v>59.3</v>
-      </c>
-      <c r="G4" s="62">
-        <v>234.5</v>
-      </c>
-      <c r="H4" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="I4" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="J4" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="126"/>
-      <c r="B5" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="62">
-        <v>4</v>
-      </c>
-      <c r="D5" s="64">
+      <c r="D25" s="55">
         <v>0.7</v>
       </c>
-      <c r="E5" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="62">
-        <v>17.5</v>
-      </c>
-      <c r="G5" s="62">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>147</v>
-      </c>
-      <c r="I5" s="67" t="s">
-        <v>137</v>
-      </c>
-      <c r="J5" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="127" t="s">
+      <c r="E25" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="111" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="58"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A26" s="121"/>
+      <c r="B26" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="53">
+        <v>1</v>
+      </c>
+      <c r="D26" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="I26" s="58"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A27" s="122"/>
+      <c r="B27" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="68" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="69">
-        <v>4</v>
-      </c>
-      <c r="D6" s="70">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E6" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="69">
-        <v>89.6</v>
-      </c>
-      <c r="G6" s="69">
-        <v>363</v>
-      </c>
-      <c r="H6" s="74" t="s">
-        <v>149</v>
-      </c>
-      <c r="I6" s="72" t="s">
-        <v>139</v>
-      </c>
-      <c r="J6" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="128"/>
-      <c r="B7" s="68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="69">
-        <v>4</v>
-      </c>
-      <c r="D7" s="70">
+      <c r="C27" s="53">
+        <v>1</v>
+      </c>
+      <c r="D27" s="55">
         <v>0.7</v>
       </c>
-      <c r="E7" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="69">
-        <v>20.8</v>
-      </c>
-      <c r="G7" s="69">
-        <v>83</v>
-      </c>
-      <c r="H7" s="74" t="s">
-        <v>150</v>
-      </c>
-      <c r="I7" s="72" t="s">
-        <v>138</v>
-      </c>
-      <c r="J7" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="129"/>
-      <c r="B8" s="68" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="69">
-        <v>4</v>
-      </c>
-      <c r="D8" s="70">
+      <c r="E27" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="111" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="58"/>
+    </row>
+    <row r="28" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A28" s="112"/>
+      <c r="B28" s="100" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="100">
+        <v>1</v>
+      </c>
+      <c r="D28" s="101">
         <v>0.7</v>
       </c>
-      <c r="E8" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="69">
-        <v>30.8</v>
-      </c>
-      <c r="G8" s="69">
-        <v>123.5</v>
-      </c>
-      <c r="H8" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="I8" s="83" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="37">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="122" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" s="63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="62">
-        <v>2</v>
-      </c>
-      <c r="D9" s="64">
-        <v>0.75</v>
-      </c>
-      <c r="E9" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="62">
-        <v>66</v>
-      </c>
-      <c r="G9" s="62">
-        <v>132</v>
-      </c>
-      <c r="H9" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="I9" s="67" t="s">
-        <v>165</v>
-      </c>
-      <c r="J9" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="123"/>
-      <c r="B10" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="62">
-        <v>2</v>
-      </c>
-      <c r="D10" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E10" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="G10" s="62">
-        <v>110.6</v>
-      </c>
-      <c r="H10" s="66" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" s="67" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="123"/>
-      <c r="B11" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="62">
-        <v>2</v>
-      </c>
-      <c r="D11" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E11" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="62">
-        <v>105</v>
-      </c>
-      <c r="H11" s="66" t="s">
-        <v>144</v>
-      </c>
-      <c r="I11" s="67" t="s">
-        <v>246</v>
-      </c>
-      <c r="J11" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="124"/>
-      <c r="B12" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="62">
-        <v>1</v>
-      </c>
-      <c r="D12" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E12" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="62">
-        <v>12</v>
-      </c>
-      <c r="H12" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="I12" s="67" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="127" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="69">
-        <v>2</v>
-      </c>
-      <c r="D13" s="70">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="69" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="I13" s="72" t="s">
-        <v>248</v>
-      </c>
-      <c r="J13" s="37">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="128"/>
-      <c r="B14" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="69">
-        <v>1</v>
-      </c>
-      <c r="D14" s="70">
-        <v>0.6</v>
-      </c>
-      <c r="E14" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="G14" s="69">
-        <v>39</v>
-      </c>
-      <c r="H14" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="I14" s="72" t="s">
-        <v>246</v>
-      </c>
-      <c r="J14" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="128"/>
-      <c r="B15" s="68" t="s">
-        <v>160</v>
-      </c>
-      <c r="C15" s="69">
-        <v>1</v>
-      </c>
-      <c r="D15" s="70">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="71" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="H15" s="74" t="s">
-        <v>161</v>
-      </c>
-      <c r="I15" s="72" t="s">
-        <v>248</v>
-      </c>
-      <c r="J15" s="37">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="128"/>
-      <c r="B16" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="76">
-        <v>1</v>
-      </c>
-      <c r="D16" s="77">
-        <v>0.7</v>
-      </c>
-      <c r="E16" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="76" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="76">
-        <v>5.7</v>
-      </c>
-      <c r="H16" s="79" t="s">
-        <v>157</v>
-      </c>
-      <c r="I16" s="80"/>
-    </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="129"/>
-      <c r="B17" s="68" t="s">
-        <v>154</v>
-      </c>
-      <c r="C17" s="69">
-        <v>1</v>
-      </c>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="81" t="s">
-        <v>156</v>
-      </c>
-      <c r="I17" s="82" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="122" t="s">
-        <v>198</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="62">
-        <v>4</v>
-      </c>
-      <c r="D18" s="64">
-        <v>0.6</v>
-      </c>
-      <c r="E18" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="62" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="62">
-        <v>148.1</v>
-      </c>
-      <c r="H18" s="66" t="s">
-        <v>162</v>
-      </c>
-      <c r="I18" s="67"/>
-    </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="124"/>
-      <c r="B19" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="62">
-        <v>4</v>
-      </c>
-      <c r="D19" s="64">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="62">
-        <v>31.8</v>
-      </c>
-      <c r="G19" s="62">
-        <v>127.1</v>
-      </c>
-      <c r="H19" s="66" t="s">
-        <v>163</v>
-      </c>
-      <c r="I19" s="67"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="111" t="s">
-        <v>251</v>
-      </c>
-      <c r="B20" s="111" t="s">
-        <v>250</v>
-      </c>
-      <c r="C20" s="111">
-        <v>8</v>
-      </c>
-      <c r="D20" s="112">
-        <v>0.4</v>
-      </c>
-      <c r="E20" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" s="111"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="74" t="s">
-        <v>252</v>
-      </c>
-      <c r="I20" s="72" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="122" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="113" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="114">
-        <v>2</v>
-      </c>
-      <c r="D21" s="115">
-        <v>0.7</v>
-      </c>
-      <c r="E21" s="116" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="114" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="114" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="117" t="s">
-        <v>164</v>
-      </c>
-      <c r="I21" s="118"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="123"/>
-      <c r="B22" s="63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C22" s="62">
-        <v>1</v>
-      </c>
-      <c r="D22" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E22" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="119" t="s">
-        <v>143</v>
-      </c>
-      <c r="I22" s="67" t="s">
-        <v>249</v>
-      </c>
-      <c r="J22" s="108">
-        <v>0.4</v>
-      </c>
-      <c r="K22" s="30"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" ht="33">
-      <c r="A23" s="123"/>
-      <c r="B23" s="63" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" s="62">
-        <v>1</v>
-      </c>
-      <c r="D23" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E23" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="120" t="s">
-        <v>159</v>
-      </c>
-      <c r="I23" s="67"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1">
-      <c r="A24" s="123"/>
-      <c r="B24" s="63" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="62">
-        <v>1</v>
-      </c>
-      <c r="D24" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E24" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="120" t="s">
-        <v>197</v>
-      </c>
-      <c r="I24" s="67"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" spans="1:12" ht="33">
-      <c r="A25" s="124"/>
-      <c r="B25" s="63" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="62">
-        <v>1</v>
-      </c>
-      <c r="D25" s="64">
-        <v>0.7</v>
-      </c>
-      <c r="E25" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="120" t="s">
-        <v>204</v>
-      </c>
-      <c r="I25" s="67"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="121"/>
-      <c r="B26" s="109" t="s">
-        <v>224</v>
-      </c>
-      <c r="C26" s="109">
-        <v>1</v>
-      </c>
-      <c r="D26" s="110">
-        <v>0.7</v>
-      </c>
-      <c r="E26" s="65" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="109"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
+      <c r="E28" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="100"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A21:A25"/>
+  <mergeCells count="7">
+    <mergeCell ref="A23:A27"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -3204,395 +3262,427 @@
     <hyperlink ref="E10" r:id="rId7" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E11" r:id="rId8" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E13" r:id="rId9"/>
-    <hyperlink ref="E21" r:id="rId10"/>
+    <hyperlink ref="E23" r:id="rId10"/>
     <hyperlink ref="E14" r:id="rId11"/>
     <hyperlink ref="E12" r:id="rId12"/>
     <hyperlink ref="E16" r:id="rId13" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E18" r:id="rId14" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
     <hyperlink ref="E19" r:id="rId15" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E22" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
+    <hyperlink ref="E24" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
     <hyperlink ref="E17" r:id="rId17"/>
-    <hyperlink ref="E23" r:id="rId18"/>
-    <hyperlink ref="E24" r:id="rId19"/>
+    <hyperlink ref="E25" r:id="rId18"/>
+    <hyperlink ref="E26" r:id="rId19"/>
     <hyperlink ref="E15" r:id="rId20" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
-    <hyperlink ref="E25" r:id="rId21"/>
-    <hyperlink ref="E26" r:id="rId22"/>
+    <hyperlink ref="E27" r:id="rId21"/>
+    <hyperlink ref="E28" r:id="rId22"/>
     <hyperlink ref="E20" r:id="rId23"/>
+    <hyperlink ref="E21" r:id="rId24"/>
+    <hyperlink ref="E22" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A25"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>87</v>
+      <c r="D1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="13">
         <v>8500</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>191</v>
+      <c r="E2" s="32" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="14">
         <v>15000</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>191</v>
+      <c r="E3" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="14">
         <f>2900*3</f>
         <v>8700</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" s="25">
+      <c r="B5" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="14">
         <v>14000</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>191</v>
+      <c r="E5" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="44" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="25">
+      <c r="B6" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="14">
         <f>1500*4</f>
         <v>6000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="D7" s="23">
+      <c r="B7" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="14">
         <f>1500*4</f>
         <v>6000</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="25">
+      <c r="B8" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="16">
         <v>53</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="14">
         <f>6*2000</f>
         <v>12000</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="14">
+        <v>23400</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D9" s="23">
-        <v>23400</v>
-      </c>
-      <c r="E9" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>5</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="14">
         <f>5*15500</f>
         <v>77500</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="23">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>176</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="A11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="6">
         <v>1</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="14">
         <v>15000</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="10">
+      <c r="B12" s="34"/>
+      <c r="C12" s="6">
         <v>1</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="32" t="s">
-        <v>191</v>
+      <c r="D12" s="14"/>
+      <c r="E12" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="32"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="32" t="s">
-        <v>191</v>
+      <c r="D14" s="14"/>
+      <c r="E14" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="10">
+      <c r="B15" s="34"/>
+      <c r="C15" s="6">
         <v>4</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="32" t="s">
-        <v>191</v>
+      <c r="D15" s="14"/>
+      <c r="E15" s="23" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="36"/>
+      <c r="C16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="42" t="s">
-        <v>191</v>
+      <c r="D16" s="15"/>
+      <c r="E16" s="33" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="D17" s="26">
+      <c r="D17" s="17">
         <f>SUM(D2:D16)</f>
         <v>186100</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="B18" s="30"/>
+      <c r="D18" s="30"/>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="B19" s="117" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="113"/>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="11">
+        <v>258</v>
+      </c>
+      <c r="B20" s="117"/>
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="10">
+      <c r="D20" s="118"/>
+      <c r="E20" s="113"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="E21" s="119"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="116" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="119"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B23" s="115" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="9">
         <v>1</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="10">
+      <c r="D23" s="118">
+        <f>26.28*1200</f>
+        <v>31536</v>
+      </c>
+      <c r="E23" s="113">
         <v>1</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="10">
+    </row>
+    <row r="24" spans="1:5">
+      <c r="E24" s="119"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="116" t="s">
+        <v>253</v>
+      </c>
+      <c r="E25" s="119"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.5">
+      <c r="A26" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" s="115" t="s">
+        <v>252</v>
+      </c>
+      <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
+      <c r="D26" s="118">
+        <f>38.5*1200</f>
+        <v>46200</v>
+      </c>
+      <c r="E26" s="113"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="E27" s="119"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="116" t="s">
+        <v>257</v>
+      </c>
+      <c r="E28" s="119"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.5">
+      <c r="A29" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B29" s="115" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="118">
+        <f>16.99*1200</f>
+        <v>20387.999999999996</v>
+      </c>
+      <c r="E29" s="113"/>
+    </row>
+    <row r="39" spans="4:4">
+      <c r="D39" s="17">
+        <f>SUM(D19:D38)</f>
+        <v>98124</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
-    <hyperlink ref="B22" r:id="rId3"/>
-    <hyperlink ref="B23" r:id="rId4"/>
-    <hyperlink ref="B24" r:id="rId5"/>
+    <hyperlink ref="B19" r:id="rId2"/>
+    <hyperlink ref="B23" r:id="rId3"/>
+    <hyperlink ref="B26" r:id="rId4"/>
+    <hyperlink ref="B29" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <drawing r:id="rId7"/>
 </worksheet>
 </file>
@@ -3608,549 +3698,549 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.375" customWidth="1"/>
-    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="59"/>
+      <c r="F1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="A2" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="13">
         <v>1500</v>
       </c>
-      <c r="G2" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="58"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>129</v>
+      <c r="G2" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="49"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="130" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="137" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="22">
+      <c r="A3" s="131" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="138" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="13">
         <v>1500</v>
       </c>
-      <c r="G3" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="58"/>
-      <c r="J3" s="135" t="s">
-        <v>133</v>
-      </c>
-      <c r="K3" s="28" t="s">
+      <c r="G3" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="49"/>
+      <c r="J3" s="136" t="s">
         <v>125</v>
       </c>
-      <c r="L3" s="34">
+      <c r="K3" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="25">
         <v>40</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="25">
         <f>L3/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="131"/>
-      <c r="B4" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="138"/>
-      <c r="E4" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="23">
+      <c r="A4" s="132"/>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="139"/>
+      <c r="E4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="14">
         <v>1500</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" s="34">
+      <c r="G4" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="49"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="25">
         <v>40</v>
       </c>
-      <c r="M4" s="34">
+      <c r="M4" s="25">
         <f t="shared" ref="M4:M5" si="0">L4/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="131"/>
-      <c r="B5" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="138"/>
-      <c r="E5" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="A5" s="132"/>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="139"/>
+      <c r="E5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="14">
         <v>1500</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="49"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="I5" s="58"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" s="34">
+      <c r="L5" s="25">
         <v>25</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="25">
         <f t="shared" si="0"/>
         <v>9.8425196850393704</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="131"/>
-      <c r="B6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="138"/>
-      <c r="E6" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="A6" s="132"/>
+      <c r="B6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="139"/>
+      <c r="E6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="14">
         <v>1500</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
+      <c r="G6" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" s="49"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="132"/>
-      <c r="B7" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="139"/>
-      <c r="E7" s="11">
+      <c r="A7" s="133"/>
+      <c r="B7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="140"/>
+      <c r="E7" s="7">
         <v>28</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="15">
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="G7" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="135" t="s">
-        <v>134</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="L7" s="34">
+      <c r="G7" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="49"/>
+      <c r="J7" s="136" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="25">
         <f>L3+27</f>
         <v>67</v>
       </c>
-      <c r="M7" s="34">
+      <c r="M7" s="25">
         <f>L7/2.54</f>
         <v>26.377952755905511</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="133" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="50">
+      <c r="A8" s="134" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="41">
         <v>1500</v>
       </c>
-      <c r="G8" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="H8" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="135"/>
-      <c r="K8" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="L8" s="34">
+      <c r="G8" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" s="49"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="25">
         <f>L4+27</f>
         <v>67</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="25">
         <f>L8/2.54</f>
         <v>26.377952755905511</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="134"/>
-      <c r="B9" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="E9" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="54">
+      <c r="A9" s="135"/>
+      <c r="B9" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="45">
         <v>1500</v>
       </c>
-      <c r="G9" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="135"/>
-      <c r="K9" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="L9" s="34">
+      <c r="G9" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="49"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="25">
         <f>L5+20</f>
         <v>45</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="25">
         <f>L9/2.54</f>
         <v>17.716535433070867</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="130" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="137" t="s">
-        <v>180</v>
-      </c>
-      <c r="E10" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="22">
+      <c r="A10" s="131" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="138" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="13">
         <f>2*1500</f>
         <v>3000</v>
       </c>
-      <c r="G10" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="I10" s="58"/>
+      <c r="G10" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="131"/>
-      <c r="B11" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="138"/>
-      <c r="E11" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="A11" s="132"/>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="139"/>
+      <c r="E11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="14">
         <v>1500</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="58"/>
-      <c r="J11" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="L11" s="34">
+      <c r="G11" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="L11" s="25">
         <f>2.54*M11</f>
         <v>39.92</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="25">
         <f>M9-2</f>
         <v>15.716535433070867</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="132"/>
-      <c r="B12" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="139"/>
-      <c r="E12" s="11">
+      <c r="A12" s="133"/>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="140"/>
+      <c r="E12" s="7">
         <v>36</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="37">
         <v>1500</v>
       </c>
-      <c r="G12" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="58"/>
+      <c r="G12" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="I12" s="49"/>
     </row>
     <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="130" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="137" t="s">
-        <v>182</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="22">
+      <c r="A13" s="131" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="138" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="13">
         <v>1500</v>
       </c>
-      <c r="G13" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="58"/>
+      <c r="G13" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="49"/>
     </row>
     <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="131"/>
-      <c r="B14" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="138"/>
-      <c r="E14" s="10">
+      <c r="A14" s="132"/>
+      <c r="B14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="139"/>
+      <c r="E14" s="6">
         <v>34</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="14">
         <v>3000</v>
       </c>
-      <c r="G14" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" s="58"/>
+      <c r="G14" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="49"/>
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="132"/>
-      <c r="B15" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="139"/>
-      <c r="E15" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" s="24">
+      <c r="A15" s="133"/>
+      <c r="B15" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="140"/>
+      <c r="E15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="15">
         <v>1500</v>
       </c>
-      <c r="G15" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="6"/>
+      <c r="G15" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="130" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="60"/>
-      <c r="E16" s="47" t="s">
+      <c r="A16" s="131" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="E16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="58"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="49"/>
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="132"/>
-      <c r="B17" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11" t="s">
+      <c r="A17" s="133"/>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="58"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="49"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="B18" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="26">
+      <c r="B18" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="17">
         <f>SUM(F2:F15)</f>
         <v>25500</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="48"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="B19" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="56"/>
+      <c r="B19" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="47"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="E27" s="6"/>
-      <c r="F27" s="30"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="44" ht="16.5" customHeight="1"/>
   </sheetData>
@@ -4171,7 +4261,7 @@
     <hyperlink ref="B19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="36" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
@@ -4184,11 +4274,11 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="46" spans="1:1">
-      <c r="A46" s="31" t="s">
-        <v>114</v>
+      <c r="A46" s="22" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4209,11 +4299,11 @@
       <selection activeCell="AJ38" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="54" spans="1:1">
-      <c r="A54" s="31" t="s">
-        <v>116</v>
+      <c r="A54" s="22" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -4234,11 +4324,11 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="55" spans="1:1">
-      <c r="A55" s="31" t="s">
-        <v>115</v>
+      <c r="A55" s="22" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4259,11 +4349,11 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="31" t="s">
-        <v>117</v>
+      <c r="A1" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -4272,7 +4362,7 @@
     <hyperlink ref="A1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
@@ -4282,344 +4372,344 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:M5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
-    <col min="2" max="2" width="37.625" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="19" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="19" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.25">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:19" ht="18.75">
+      <c r="A1" s="84" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="84" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="84" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="141" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="78" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="31">
+        <v>4</v>
+      </c>
+      <c r="D2" s="143">
+        <v>4</v>
+      </c>
+      <c r="E2" s="143">
+        <v>6</v>
+      </c>
+      <c r="H2" s="85">
+        <v>1</v>
+      </c>
+      <c r="I2" s="85">
+        <v>2</v>
+      </c>
+      <c r="J2" s="85">
+        <v>3</v>
+      </c>
+      <c r="K2" s="85">
+        <v>4</v>
+      </c>
+      <c r="L2" s="85">
+        <v>5</v>
+      </c>
+      <c r="M2" s="85">
+        <v>6</v>
+      </c>
+      <c r="N2" s="82">
+        <v>7</v>
+      </c>
+      <c r="O2" s="82">
+        <v>8</v>
+      </c>
+      <c r="P2" s="82">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="82">
+        <v>10</v>
+      </c>
+      <c r="R2" s="82">
+        <v>11</v>
+      </c>
+      <c r="S2" s="82">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="142"/>
+      <c r="B3" s="78" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="31">
+        <v>2</v>
+      </c>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="H3" s="85" t="s">
+        <v>211</v>
+      </c>
+      <c r="I3" s="85" t="s">
+        <v>212</v>
+      </c>
+      <c r="J3" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="93" t="s">
+      <c r="K3" s="85" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="L3" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="93" t="s">
-        <v>216</v>
-      </c>
-      <c r="E1" s="93" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="140" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="87" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="40">
-        <v>4</v>
-      </c>
-      <c r="D2" s="142">
-        <v>4</v>
-      </c>
-      <c r="E2" s="142">
-        <v>6</v>
-      </c>
-      <c r="H2" s="94">
+      <c r="M3" s="85" t="s">
+        <v>215</v>
+      </c>
+      <c r="N3" s="82" t="s">
+        <v>202</v>
+      </c>
+      <c r="O3" s="82"/>
+      <c r="P3" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q3" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="R3" s="97" t="s">
+        <v>233</v>
+      </c>
+      <c r="S3" s="98" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="142"/>
+      <c r="B4" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="31">
         <v>1</v>
       </c>
-      <c r="I2" s="94">
+      <c r="D4" s="144"/>
+      <c r="E4" s="144"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="92"/>
+      <c r="S4" s="89"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="142"/>
+      <c r="B5" s="94" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1</v>
+      </c>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="142"/>
+      <c r="B6" s="87" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="76">
+        <v>1</v>
+      </c>
+      <c r="D6" s="144"/>
+      <c r="E6" s="144"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="142"/>
+      <c r="B7" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="76">
+        <v>1</v>
+      </c>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="141" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="88" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="77">
+        <v>1</v>
+      </c>
+      <c r="D8" s="143">
         <v>2</v>
       </c>
-      <c r="J2" s="94">
-        <v>3</v>
-      </c>
-      <c r="K2" s="94">
-        <v>4</v>
-      </c>
-      <c r="L2" s="94">
-        <v>5</v>
-      </c>
-      <c r="M2" s="94">
-        <v>6</v>
-      </c>
-      <c r="N2" s="91">
-        <v>7</v>
-      </c>
-      <c r="O2" s="91">
-        <v>8</v>
-      </c>
-      <c r="P2" s="91">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="91">
-        <v>10</v>
-      </c>
-      <c r="R2" s="91">
-        <v>11</v>
-      </c>
-      <c r="S2" s="91">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="141"/>
-      <c r="B3" s="87" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="40">
-        <v>2</v>
-      </c>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="H3" s="94" t="s">
+      <c r="E8" s="143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="142"/>
+      <c r="B9" s="80" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="77">
+        <v>1</v>
+      </c>
+      <c r="D9" s="144"/>
+      <c r="E9" s="144"/>
+      <c r="H9" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="94" t="s">
-        <v>220</v>
-      </c>
-      <c r="J3" s="94" t="s">
-        <v>221</v>
-      </c>
-      <c r="K3" s="94" t="s">
-        <v>222</v>
-      </c>
-      <c r="L3" s="94" t="s">
-        <v>223</v>
-      </c>
-      <c r="M3" s="94" t="s">
-        <v>223</v>
-      </c>
-      <c r="N3" s="91" t="s">
-        <v>210</v>
-      </c>
-      <c r="O3" s="91"/>
-      <c r="P3" s="104" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q3" s="105" t="s">
-        <v>239</v>
-      </c>
-      <c r="R3" s="106" t="s">
-        <v>241</v>
-      </c>
-      <c r="S3" s="107" t="s">
+      <c r="J9" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="141"/>
-      <c r="B4" s="102" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="40">
-        <v>1</v>
-      </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="98"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="101"/>
-      <c r="S4" s="98"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="141"/>
-      <c r="B5" s="103" t="s">
-        <v>243</v>
-      </c>
-      <c r="C5" s="40">
-        <v>1</v>
-      </c>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="141"/>
-      <c r="B6" s="96" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="85">
-        <v>1</v>
-      </c>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="141"/>
-      <c r="B7" s="88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C7" s="85">
-        <v>1</v>
-      </c>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="140" t="s">
-        <v>209</v>
-      </c>
-      <c r="B8" s="97" t="s">
-        <v>245</v>
-      </c>
-      <c r="C8" s="86">
-        <v>1</v>
-      </c>
-      <c r="D8" s="142">
-        <v>2</v>
-      </c>
-      <c r="E8" s="142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="141"/>
-      <c r="B9" s="89" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="86">
-        <v>1</v>
-      </c>
-      <c r="D9" s="143"/>
-      <c r="E9" s="143"/>
-      <c r="H9" t="s">
-        <v>227</v>
-      </c>
-      <c r="J9" t="s">
-        <v>226</v>
-      </c>
-      <c r="K9" s="95">
+      <c r="K9" s="86">
         <v>390</v>
       </c>
       <c r="L9">
         <v>2</v>
       </c>
-      <c r="M9" s="95">
+      <c r="M9" s="86">
         <f t="shared" ref="M9:M14" si="0">K9*L9</f>
         <v>780</v>
       </c>
-      <c r="N9" s="31" t="s">
-        <v>225</v>
+      <c r="N9" s="22" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="145"/>
-      <c r="B10" s="90" t="s">
-        <v>210</v>
-      </c>
-      <c r="C10" s="36">
+      <c r="A10" s="146"/>
+      <c r="B10" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="27">
         <v>1</v>
       </c>
-      <c r="D10" s="144"/>
-      <c r="E10" s="144"/>
-      <c r="K10" s="95"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="31"/>
+      <c r="D10" s="145"/>
+      <c r="E10" s="145"/>
+      <c r="K10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="22"/>
     </row>
     <row r="11" spans="1:19">
       <c r="H11" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="J11" t="s">
-        <v>229</v>
-      </c>
-      <c r="K11" s="95">
+        <v>221</v>
+      </c>
+      <c r="K11" s="86">
         <v>500</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" s="95">
+      <c r="M11" s="86">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="N11" s="31" t="s">
-        <v>228</v>
+      <c r="N11" s="22" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="91" t="s">
-        <v>211</v>
-      </c>
-      <c r="B13" s="92" t="s">
-        <v>212</v>
-      </c>
-      <c r="C13" s="91">
+      <c r="A13" s="82" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="82">
         <v>2</v>
       </c>
-      <c r="D13" s="91">
+      <c r="D13" s="82">
         <v>0</v>
       </c>
-      <c r="E13" s="91">
+      <c r="E13" s="82">
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="J13" t="s">
-        <v>232</v>
-      </c>
-      <c r="K13" s="95">
+        <v>224</v>
+      </c>
+      <c r="K13" s="86">
         <v>210</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="M13" s="95">
+      <c r="M13" s="86">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="N13" s="31" t="s">
-        <v>236</v>
+      <c r="N13" s="22" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="H14" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="J14" t="s">
-        <v>231</v>
-      </c>
-      <c r="K14" s="95">
+        <v>223</v>
+      </c>
+      <c r="K14" s="86">
         <v>510</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
-      <c r="M14" s="95">
+      <c r="M14" s="86">
         <f t="shared" si="0"/>
         <v>510</v>
       </c>
-      <c r="N14" s="31" t="s">
-        <v>233</v>
+      <c r="N14" s="22" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="H15" t="s">
-        <v>238</v>
-      </c>
-      <c r="K15" s="95">
+        <v>230</v>
+      </c>
+      <c r="K15" s="86">
         <v>50</v>
       </c>
       <c r="L15">
         <v>20</v>
       </c>
-      <c r="M15" s="95">
+      <c r="M15" s="86">
         <f>K15*L15</f>
         <v>1000</v>
       </c>
-      <c r="N15" s="31" t="s">
-        <v>237</v>
+      <c r="N15" s="22" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drag chain holder added
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\Mostly-Printed-CNC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\03.Mostly-Printed-CNC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="261">
   <si>
     <t>QTY</t>
   </si>
@@ -870,22 +870,38 @@
   <si>
     <t>Z-END</t>
   </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>drag chain holder</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPCNCdragchain.stl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="166" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="167" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
   </numFmts>
   <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -914,14 +930,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -942,7 +958,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -951,7 +967,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -960,7 +976,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -998,14 +1014,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1020,7 +1036,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1028,14 +1044,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1043,7 +1059,7 @@
     <font>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1052,7 +1068,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1060,7 +1076,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1068,7 +1084,7 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1359,19 +1375,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,7 +1399,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -1434,7 +1450,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1443,7 +1459,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1527,7 +1543,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1563,7 +1579,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1653,7 +1669,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1692,10 +1708,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1704,22 +1720,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1737,10 +1753,10 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1749,6 +1765,30 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1758,49 +1798,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1818,6 +1819,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1838,8 +1854,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2308,7 +2324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2570,22 +2586,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="2" max="2" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2623,7 +2639,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="151" t="s">
+      <c r="A4" s="143" t="s">
         <v>157</v>
       </c>
       <c r="B4" s="70" t="s">
@@ -2655,7 +2671,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="152"/>
+      <c r="A5" s="144"/>
       <c r="B5" s="49" t="s">
         <v>78</v>
       </c>
@@ -2685,7 +2701,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A6" s="153" t="s">
+      <c r="A6" s="145" t="s">
         <v>158</v>
       </c>
       <c r="B6" s="54" t="s">
@@ -2717,7 +2733,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A7" s="154"/>
+      <c r="A7" s="146"/>
       <c r="B7" s="54" t="s">
         <v>7</v>
       </c>
@@ -2747,7 +2763,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A8" s="155"/>
+      <c r="A8" s="147"/>
       <c r="B8" s="54" t="s">
         <v>8</v>
       </c>
@@ -2777,7 +2793,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A9" s="146" t="s">
+      <c r="A9" s="148" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="49" t="s">
@@ -2809,7 +2825,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A10" s="147"/>
+      <c r="A10" s="149"/>
       <c r="B10" s="49" t="s">
         <v>10</v>
       </c>
@@ -2839,7 +2855,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A11" s="147"/>
+      <c r="A11" s="149"/>
       <c r="B11" s="49" t="s">
         <v>11</v>
       </c>
@@ -2869,7 +2885,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A12" s="148"/>
+      <c r="A12" s="150"/>
       <c r="B12" s="49" t="s">
         <v>17</v>
       </c>
@@ -2899,7 +2915,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A13" s="153" t="s">
+      <c r="A13" s="145" t="s">
         <v>160</v>
       </c>
       <c r="B13" s="54" t="s">
@@ -2931,7 +2947,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A14" s="154"/>
+      <c r="A14" s="146"/>
       <c r="B14" s="54" t="s">
         <v>16</v>
       </c>
@@ -2961,7 +2977,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A15" s="154"/>
+      <c r="A15" s="146"/>
       <c r="B15" s="54" t="s">
         <v>127</v>
       </c>
@@ -2991,7 +3007,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A16" s="154"/>
+      <c r="A16" s="146"/>
       <c r="B16" s="61" t="s">
         <v>19</v>
       </c>
@@ -3016,7 +3032,7 @@
       <c r="I16" s="66"/>
     </row>
     <row r="17" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A17" s="155"/>
+      <c r="A17" s="147"/>
       <c r="B17" s="54" t="s">
         <v>122</v>
       </c>
@@ -3037,7 +3053,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A18" s="146" t="s">
+      <c r="A18" s="148" t="s">
         <v>161</v>
       </c>
       <c r="B18" s="49" t="s">
@@ -3069,7 +3085,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A19" s="148"/>
+      <c r="A19" s="150"/>
       <c r="B19" s="49" t="s">
         <v>75</v>
       </c>
@@ -3099,7 +3115,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="151" t="s">
         <v>154</v>
       </c>
       <c r="B20" s="95" t="s">
@@ -3127,7 +3143,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A21" s="144"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="95" t="s">
         <v>201</v>
       </c>
@@ -3153,8 +3169,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A22" s="144"/>
-      <c r="B22" s="143" t="s">
+      <c r="A22" s="152"/>
+      <c r="B22" s="151" t="s">
         <v>204</v>
       </c>
       <c r="C22" s="95">
@@ -3171,11 +3187,16 @@
       <c r="H22" s="107" t="s">
         <v>245</v>
       </c>
-      <c r="I22" s="58"/>
+      <c r="I22" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="J22" s="27">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A23" s="144"/>
-      <c r="B23" s="144"/>
+      <c r="A23" s="152"/>
+      <c r="B23" s="152"/>
       <c r="C23" s="95">
         <v>1</v>
       </c>
@@ -3190,11 +3211,16 @@
       <c r="H23" s="107" t="s">
         <v>246</v>
       </c>
-      <c r="I23" s="58"/>
+      <c r="I23" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="J23" s="27">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A24" s="145"/>
-      <c r="B24" s="145"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="153"/>
       <c r="C24" s="95">
         <v>1</v>
       </c>
@@ -3209,70 +3235,73 @@
       <c r="H24" s="107" t="s">
         <v>247</v>
       </c>
-      <c r="I24" s="58"/>
+      <c r="I24" s="58" t="s">
+        <v>257</v>
+      </c>
+      <c r="J24" s="27">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A25" s="146" t="s">
+      <c r="A25" s="153"/>
+      <c r="B25" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="C25" s="95">
+        <v>1</v>
+      </c>
+      <c r="D25" s="96">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="95"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="107" t="s">
+        <v>260</v>
+      </c>
+      <c r="I25" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="27">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A26" s="148" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="97" t="s">
+      <c r="B26" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="98">
+      <c r="C26" s="98">
         <v>2</v>
       </c>
-      <c r="D25" s="99">
+      <c r="D26" s="99">
         <v>0.7</v>
       </c>
-      <c r="E25" s="100" t="s">
+      <c r="E26" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="98" t="s">
+      <c r="F26" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="98" t="s">
+      <c r="G26" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="101" t="s">
+      <c r="H26" s="101" t="s">
         <v>131</v>
       </c>
-      <c r="I25" s="102"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A26" s="147"/>
-      <c r="B26" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="C26" s="48">
-        <v>1</v>
-      </c>
-      <c r="D26" s="50">
-        <v>0.7</v>
-      </c>
-      <c r="E26" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="103" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="J26" s="92">
-        <v>0.4</v>
-      </c>
+      <c r="I26" s="102"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="21"/>
       <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A27" s="147"/>
-      <c r="B27" s="146" t="s">
-        <v>163</v>
+      <c r="A27" s="149"/>
+      <c r="B27" s="49" t="s">
+        <v>164</v>
       </c>
       <c r="C27" s="48">
         <v>1</v>
@@ -3285,21 +3314,23 @@
       </c>
       <c r="F27" s="48"/>
       <c r="G27" s="48"/>
-      <c r="H27" s="104" t="s">
-        <v>241</v>
+      <c r="H27" s="103" t="s">
+        <v>111</v>
       </c>
       <c r="I27" s="53" t="s">
-        <v>90</v>
+        <v>198</v>
       </c>
       <c r="J27" s="92">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="K27" s="21"/>
       <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A28" s="147"/>
-      <c r="B28" s="148"/>
+      <c r="A28" s="149"/>
+      <c r="B28" s="148" t="s">
+        <v>163</v>
+      </c>
       <c r="C28" s="48">
         <v>1</v>
       </c>
@@ -3312,7 +3343,7 @@
       <c r="F28" s="48"/>
       <c r="G28" s="48"/>
       <c r="H28" s="104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I28" s="53" t="s">
         <v>90</v>
@@ -3324,67 +3355,69 @@
       <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A29" s="147"/>
-      <c r="B29" s="146" t="s">
-        <v>166</v>
-      </c>
+      <c r="A29" s="149"/>
+      <c r="B29" s="150"/>
       <c r="C29" s="48">
         <v>1</v>
       </c>
       <c r="D29" s="50">
         <v>0.7</v>
       </c>
-      <c r="E29" s="149" t="s">
+      <c r="E29" s="51" t="s">
         <v>109</v>
       </c>
       <c r="F29" s="48"/>
       <c r="G29" s="48"/>
       <c r="H29" s="104" t="s">
-        <v>238</v>
-      </c>
-      <c r="I29" s="53"/>
-      <c r="J29" s="20"/>
+        <v>242</v>
+      </c>
+      <c r="I29" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="92">
+        <v>0.3</v>
+      </c>
       <c r="K29" s="21"/>
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A30" s="147"/>
-      <c r="B30" s="147"/>
+      <c r="A30" s="149"/>
+      <c r="B30" s="148" t="s">
+        <v>166</v>
+      </c>
       <c r="C30" s="48">
         <v>1</v>
       </c>
       <c r="D30" s="50">
         <v>0.7</v>
       </c>
-      <c r="E30" s="150"/>
+      <c r="E30" s="154" t="s">
+        <v>109</v>
+      </c>
       <c r="F30" s="48"/>
       <c r="G30" s="48"/>
       <c r="H30" s="104" t="s">
-        <v>239</v>
-      </c>
-      <c r="I30" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="92">
-        <v>0.4</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="I30" s="53"/>
+      <c r="J30" s="20"/>
       <c r="K30" s="21"/>
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A31" s="147"/>
-      <c r="B31" s="148"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="149"/>
       <c r="C31" s="48">
         <v>1</v>
       </c>
       <c r="D31" s="50">
         <v>0.7</v>
       </c>
-      <c r="E31" s="142"/>
+      <c r="E31" s="155"/>
       <c r="F31" s="48"/>
       <c r="G31" s="48"/>
       <c r="H31" s="104" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>90</v>
@@ -3396,77 +3429,101 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A32" s="147"/>
-      <c r="B32" s="146" t="s">
-        <v>165</v>
-      </c>
+      <c r="A32" s="149"/>
+      <c r="B32" s="150"/>
       <c r="C32" s="48">
         <v>1</v>
       </c>
       <c r="D32" s="50">
         <v>0.7</v>
       </c>
-      <c r="E32" s="149" t="s">
-        <v>109</v>
-      </c>
+      <c r="E32" s="142"/>
       <c r="F32" s="48"/>
       <c r="G32" s="48"/>
       <c r="H32" s="104" t="s">
-        <v>243</v>
-      </c>
-      <c r="I32" s="53"/>
+        <v>240</v>
+      </c>
+      <c r="I32" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="92">
+        <v>0.4</v>
+      </c>
+      <c r="K32" s="21"/>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:9" ht="28.5" customHeight="1">
-      <c r="A33" s="148"/>
-      <c r="B33" s="148"/>
+      <c r="A33" s="149"/>
+      <c r="B33" s="148" t="s">
+        <v>165</v>
+      </c>
       <c r="C33" s="48">
         <v>1</v>
       </c>
       <c r="D33" s="50">
         <v>0.7</v>
       </c>
-      <c r="E33" s="150"/>
+      <c r="E33" s="154" t="s">
+        <v>109</v>
+      </c>
       <c r="F33" s="48"/>
       <c r="G33" s="48"/>
       <c r="H33" s="104" t="s">
+        <v>243</v>
+      </c>
+      <c r="I33" s="53"/>
+    </row>
+    <row r="34" spans="1:9" ht="28.5" customHeight="1">
+      <c r="A34" s="150"/>
+      <c r="B34" s="150"/>
+      <c r="C34" s="48">
+        <v>1</v>
+      </c>
+      <c r="D34" s="50">
+        <v>0.7</v>
+      </c>
+      <c r="E34" s="155"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="104" t="s">
         <v>244</v>
       </c>
-      <c r="I33" s="53"/>
-    </row>
-    <row r="34" spans="1:9" ht="28.5" customHeight="1">
-      <c r="A34" s="105"/>
-      <c r="B34" s="93" t="s">
+      <c r="I34" s="53"/>
+    </row>
+    <row r="35" spans="1:9" ht="28.5" customHeight="1">
+      <c r="A35" s="105"/>
+      <c r="B35" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="93">
-        <v>1</v>
-      </c>
-      <c r="D34" s="94">
+      <c r="C35" s="93">
+        <v>1</v>
+      </c>
+      <c r="D35" s="94">
         <v>0.7</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E35" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="F34" s="93"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A26:A34"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A20:A25"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A25:A33"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A20:A24"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -3479,28 +3536,29 @@
     <hyperlink ref="E10" r:id="rId7" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E11" r:id="rId8" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E13" r:id="rId9"/>
-    <hyperlink ref="E25" r:id="rId10"/>
+    <hyperlink ref="E26" r:id="rId10"/>
     <hyperlink ref="E14" r:id="rId11"/>
     <hyperlink ref="E12" r:id="rId12"/>
     <hyperlink ref="E16" r:id="rId13" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E18" r:id="rId14" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
     <hyperlink ref="E19" r:id="rId15" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E26" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
+    <hyperlink ref="E27" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
     <hyperlink ref="E17" r:id="rId17"/>
-    <hyperlink ref="E27" r:id="rId18"/>
-    <hyperlink ref="E29" r:id="rId19"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E30" r:id="rId19"/>
     <hyperlink ref="E15" r:id="rId20" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
-    <hyperlink ref="E32" r:id="rId21"/>
-    <hyperlink ref="E34" r:id="rId22"/>
+    <hyperlink ref="E33" r:id="rId21"/>
+    <hyperlink ref="E35" r:id="rId22"/>
     <hyperlink ref="E20" r:id="rId23"/>
     <hyperlink ref="E21" r:id="rId24"/>
     <hyperlink ref="E22" r:id="rId25"/>
-    <hyperlink ref="E28" r:id="rId26"/>
+    <hyperlink ref="E29" r:id="rId26"/>
     <hyperlink ref="E23" r:id="rId27"/>
     <hyperlink ref="E24" r:id="rId28"/>
+    <hyperlink ref="E25" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
@@ -3512,15 +3570,15 @@
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4059,7 +4117,7 @@
         <v>31536</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="21">
+    <row r="32" spans="1:9" ht="26.25">
       <c r="D32" s="138" t="s">
         <v>227</v>
       </c>
@@ -4109,21 +4167,21 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.375" customWidth="1"/>
+    <col min="14" max="14" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.100000000000001" customHeight="1">
@@ -4202,7 +4260,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="161" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="35" t="s">
@@ -4211,7 +4269,7 @@
       <c r="C3" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="163" t="s">
+      <c r="D3" s="158" t="s">
         <v>148</v>
       </c>
       <c r="E3" s="35">
@@ -4235,7 +4293,7 @@
         <v>90</v>
       </c>
       <c r="K3" s="44"/>
-      <c r="L3" s="161" t="s">
+      <c r="L3" s="156" t="s">
         <v>101</v>
       </c>
       <c r="M3" s="19" t="s">
@@ -4250,14 +4308,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="157"/>
+      <c r="A4" s="162"/>
       <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="164"/>
+      <c r="D4" s="159"/>
       <c r="E4" s="6">
         <v>8</v>
       </c>
@@ -4279,7 +4337,7 @@
         <v>90</v>
       </c>
       <c r="K4" s="44"/>
-      <c r="L4" s="162"/>
+      <c r="L4" s="157"/>
       <c r="M4" s="19" t="s">
         <v>94</v>
       </c>
@@ -4292,14 +4350,14 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="157"/>
+      <c r="A5" s="162"/>
       <c r="B5" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="164"/>
+      <c r="D5" s="159"/>
       <c r="E5" s="6">
         <v>2</v>
       </c>
@@ -4321,7 +4379,7 @@
         <v>90</v>
       </c>
       <c r="K5" s="44"/>
-      <c r="L5" s="162"/>
+      <c r="L5" s="157"/>
       <c r="M5" s="19" t="s">
         <v>95</v>
       </c>
@@ -4334,14 +4392,14 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="157"/>
+      <c r="A6" s="162"/>
       <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="164"/>
+      <c r="D6" s="159"/>
       <c r="E6" s="6">
         <v>2</v>
       </c>
@@ -4369,14 +4427,14 @@
       <c r="O6" s="25"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="158"/>
+      <c r="A7" s="163"/>
       <c r="B7" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="165"/>
+      <c r="D7" s="160"/>
       <c r="E7" s="7">
         <v>28</v>
       </c>
@@ -4399,7 +4457,7 @@
         <v>90</v>
       </c>
       <c r="K7" s="44"/>
-      <c r="L7" s="161" t="s">
+      <c r="L7" s="156" t="s">
         <v>102</v>
       </c>
       <c r="M7" s="19" t="s">
@@ -4415,7 +4473,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="159" t="s">
+      <c r="A8" s="164" t="s">
         <v>151</v>
       </c>
       <c r="B8" s="36" t="s">
@@ -4448,7 +4506,7 @@
         <v>90</v>
       </c>
       <c r="K8" s="44"/>
-      <c r="L8" s="161"/>
+      <c r="L8" s="156"/>
       <c r="M8" s="19" t="s">
         <v>99</v>
       </c>
@@ -4462,7 +4520,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="160"/>
+      <c r="A9" s="165"/>
       <c r="B9" s="39" t="s">
         <v>144</v>
       </c>
@@ -4493,7 +4551,7 @@
         <v>90</v>
       </c>
       <c r="K9" s="44"/>
-      <c r="L9" s="161"/>
+      <c r="L9" s="156"/>
       <c r="M9" s="19" t="s">
         <v>100</v>
       </c>
@@ -4507,7 +4565,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="156" t="s">
+      <c r="A10" s="161" t="s">
         <v>152</v>
       </c>
       <c r="B10" s="35" t="s">
@@ -4516,7 +4574,7 @@
       <c r="C10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="163" t="s">
+      <c r="D10" s="158" t="s">
         <v>145</v>
       </c>
       <c r="E10" s="35">
@@ -4543,14 +4601,14 @@
       <c r="K10" s="44"/>
     </row>
     <row r="11" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="157"/>
+      <c r="A11" s="162"/>
       <c r="B11" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="164"/>
+      <c r="D11" s="159"/>
       <c r="E11" s="6">
         <v>3</v>
       </c>
@@ -4588,14 +4646,14 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="158"/>
+      <c r="A12" s="163"/>
       <c r="B12" s="7" t="s">
         <v>67</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="165"/>
+      <c r="D12" s="160"/>
       <c r="E12" s="7">
         <v>36</v>
       </c>
@@ -4619,7 +4677,7 @@
       <c r="K12" s="44"/>
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="161" t="s">
         <v>153</v>
       </c>
       <c r="B13" s="35" t="s">
@@ -4628,7 +4686,7 @@
       <c r="C13" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="163" t="s">
+      <c r="D13" s="158" t="s">
         <v>147</v>
       </c>
       <c r="E13" s="35">
@@ -4654,14 +4712,14 @@
       <c r="K13" s="44"/>
     </row>
     <row r="14" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="157"/>
+      <c r="A14" s="162"/>
       <c r="B14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="164"/>
+      <c r="D14" s="159"/>
       <c r="E14" s="6">
         <v>34</v>
       </c>
@@ -4685,14 +4743,14 @@
       <c r="K14" s="44"/>
     </row>
     <row r="15" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="158"/>
+      <c r="A15" s="163"/>
       <c r="B15" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="165"/>
+      <c r="D15" s="160"/>
       <c r="E15" s="7">
         <v>22</v>
       </c>
@@ -4717,7 +4775,7 @@
       <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="161" t="s">
         <v>154</v>
       </c>
       <c r="B16" s="35" t="s">
@@ -4740,7 +4798,7 @@
       <c r="K16" s="44"/>
     </row>
     <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="158"/>
+      <c r="A17" s="163"/>
       <c r="B17" s="7" t="s">
         <v>60</v>
       </c>
@@ -4898,16 +4956,16 @@
     <row r="46" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="L3:L5"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4928,8 +4986,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -4937,22 +4996,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection sqref="A1:S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="37.625" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75">
+    <row r="1" spans="1:19" ht="20.25">
       <c r="A1" s="79" t="s">
         <v>175</v>
       </c>
@@ -5303,7 +5365,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5315,7 +5377,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="46" spans="1:1">
       <c r="A46" s="22" t="s">
@@ -5340,7 +5402,7 @@
       <selection activeCell="AJ38" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="54" spans="1:1">
       <c r="A54" s="22" t="s">
@@ -5365,7 +5427,7 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="55" spans="1:1">
       <c r="A55" s="22" t="s">
@@ -5390,7 +5452,7 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="22" t="s">

</xml_diff>

<commit_message>
change Z axis to T8 lead screw
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Printed Parts" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="300">
   <si>
     <t>QTY</t>
   </si>
@@ -664,9 +664,6 @@
   <si>
     <t>IE25mm-A-endstops_XY.stl
 IE25mm-B-endstops_Z.stl</t>
-  </si>
-  <si>
-    <t>riemenhalter.stl</t>
   </si>
   <si>
     <t>RepRapDiscount Full Graphic Smart Controller</t>
@@ -871,9 +868,6 @@
   </si>
   <si>
     <t>Laser holder</t>
-  </si>
-  <si>
-    <t>holder.stl</t>
   </si>
   <si>
     <t>E-STP1</t>
@@ -1156,6 +1150,30 @@
       </rPr>
       <t>파이프</t>
     </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>belt_clip_body.stl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D printer fan duct</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Felix_E3DV5_fan_duct_V2.stl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Proximity sensor holder for Z axis end stop</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>sensor_holder_all.stl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>laser_holder.stl</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2069,6 +2087,45 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2084,37 +2141,28 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2132,21 +2180,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2164,21 +2197,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2957,10 +2975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3010,7 +3028,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="163" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="69" t="s">
@@ -3042,7 +3060,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="151"/>
+      <c r="A5" s="164"/>
       <c r="B5" s="48" t="s">
         <v>77</v>
       </c>
@@ -3072,7 +3090,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="165" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="53" t="s">
@@ -3104,7 +3122,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A7" s="153"/>
+      <c r="A7" s="166"/>
       <c r="B7" s="53" t="s">
         <v>7</v>
       </c>
@@ -3134,7 +3152,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A8" s="154"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="53" t="s">
         <v>8</v>
       </c>
@@ -3286,7 +3304,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A13" s="152" t="s">
+      <c r="A13" s="165" t="s">
         <v>155</v>
       </c>
       <c r="B13" s="53" t="s">
@@ -3318,7 +3336,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A14" s="153"/>
+      <c r="A14" s="166"/>
       <c r="B14" s="53" t="s">
         <v>16</v>
       </c>
@@ -3348,7 +3366,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A15" s="153"/>
+      <c r="A15" s="166"/>
       <c r="B15" s="53" t="s">
         <v>123</v>
       </c>
@@ -3378,7 +3396,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A16" s="153"/>
+      <c r="A16" s="166"/>
       <c r="B16" s="60" t="s">
         <v>19</v>
       </c>
@@ -3403,7 +3421,7 @@
       <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A17" s="154"/>
+      <c r="A17" s="167"/>
       <c r="B17" s="53" t="s">
         <v>119</v>
       </c>
@@ -3417,7 +3435,7 @@
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="H17" s="66" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I17" s="67" t="s">
         <v>190</v>
@@ -3486,7 +3504,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A20" s="158" t="s">
+      <c r="A20" s="152" t="s">
         <v>149</v>
       </c>
       <c r="B20" s="88" t="s">
@@ -3504,7 +3522,7 @@
       <c r="F20" s="88"/>
       <c r="G20" s="57"/>
       <c r="H20" s="59" t="s">
-        <v>193</v>
+        <v>294</v>
       </c>
       <c r="I20" s="57" t="s">
         <v>104</v>
@@ -3514,7 +3532,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A21" s="159"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="88" t="s">
         <v>191</v>
       </c>
@@ -3540,9 +3558,9 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A22" s="159"/>
-      <c r="B22" s="158" t="s">
-        <v>194</v>
+      <c r="A22" s="153"/>
+      <c r="B22" s="152" t="s">
+        <v>193</v>
       </c>
       <c r="C22" s="88">
         <v>1</v>
@@ -3556,18 +3574,18 @@
       <c r="F22" s="88"/>
       <c r="G22" s="57"/>
       <c r="H22" s="100" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I22" s="57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J22" s="26">
         <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A23" s="159"/>
-      <c r="B23" s="159"/>
+      <c r="A23" s="153"/>
+      <c r="B23" s="153"/>
       <c r="C23" s="88">
         <v>1</v>
       </c>
@@ -3580,18 +3598,18 @@
       <c r="F23" s="88"/>
       <c r="G23" s="57"/>
       <c r="H23" s="100" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I23" s="57" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J23" s="26">
         <v>0.3</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A24" s="159"/>
-      <c r="B24" s="160"/>
+      <c r="A24" s="153"/>
+      <c r="B24" s="154"/>
       <c r="C24" s="88">
         <v>1</v>
       </c>
@@ -3604,19 +3622,19 @@
       <c r="F24" s="88"/>
       <c r="G24" s="57"/>
       <c r="H24" s="100" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I24" s="57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J24" s="26">
         <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A25" s="159"/>
+      <c r="A25" s="153"/>
       <c r="B25" s="88" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C25" s="88">
         <v>1</v>
@@ -3630,7 +3648,7 @@
       <c r="F25" s="88"/>
       <c r="G25" s="57"/>
       <c r="H25" s="100" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I25" s="57" t="s">
         <v>88</v>
@@ -3640,9 +3658,9 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A26" s="159"/>
-      <c r="B26" s="158" t="s">
-        <v>251</v>
+      <c r="A26" s="153"/>
+      <c r="B26" s="152" t="s">
+        <v>250</v>
       </c>
       <c r="C26" s="88">
         <v>1</v>
@@ -3650,13 +3668,13 @@
       <c r="D26" s="89">
         <v>0.5</v>
       </c>
-      <c r="E26" s="163" t="s">
+      <c r="E26" s="160" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="88"/>
       <c r="G26" s="57"/>
       <c r="H26" s="100" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I26" s="57" t="s">
         <v>88</v>
@@ -3666,19 +3684,19 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A27" s="159"/>
-      <c r="B27" s="159"/>
+      <c r="A27" s="153"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="88">
         <v>1</v>
       </c>
       <c r="D27" s="89">
         <v>0.5</v>
       </c>
-      <c r="E27" s="164"/>
+      <c r="E27" s="161"/>
       <c r="F27" s="88"/>
       <c r="G27" s="57"/>
       <c r="H27" s="100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I27" s="57" t="s">
         <v>88</v>
@@ -3688,19 +3706,19 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A28" s="160"/>
-      <c r="B28" s="160"/>
+      <c r="A28" s="153"/>
+      <c r="B28" s="154"/>
       <c r="C28" s="88">
         <v>1</v>
       </c>
       <c r="D28" s="89">
         <v>0.5</v>
       </c>
-      <c r="E28" s="165"/>
+      <c r="E28" s="162"/>
       <c r="F28" s="88"/>
       <c r="G28" s="57"/>
       <c r="H28" s="100" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I28" s="57" t="s">
         <v>88</v>
@@ -3710,94 +3728,90 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A29" s="155" t="s">
+      <c r="A29" s="153"/>
+      <c r="B29" s="88" t="s">
+        <v>295</v>
+      </c>
+      <c r="C29" s="88">
+        <v>1</v>
+      </c>
+      <c r="D29" s="89">
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="88"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="100" t="s">
+        <v>296</v>
+      </c>
+      <c r="I29" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="J29" s="26">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A30" s="154"/>
+      <c r="B30" s="88" t="s">
+        <v>297</v>
+      </c>
+      <c r="C30" s="88">
+        <v>1</v>
+      </c>
+      <c r="D30" s="89">
+        <v>0.3</v>
+      </c>
+      <c r="E30" s="56"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="100" t="s">
+        <v>298</v>
+      </c>
+      <c r="I30" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" s="26">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A31" s="155" t="s">
         <v>162</v>
       </c>
-      <c r="B29" s="90" t="s">
+      <c r="B31" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="91">
+      <c r="C31" s="91">
         <v>2</v>
       </c>
-      <c r="D29" s="92">
+      <c r="D31" s="92">
         <v>0.7</v>
       </c>
-      <c r="E29" s="93" t="s">
+      <c r="E31" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="91" t="s">
+      <c r="F31" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="G29" s="91" t="s">
+      <c r="G31" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="94" t="s">
+      <c r="H31" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="I29" s="95"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A30" s="156"/>
-      <c r="B30" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="47">
-        <v>1</v>
-      </c>
-      <c r="D30" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="E30" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="96" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" s="52" t="s">
-        <v>188</v>
-      </c>
-      <c r="J30" s="85">
-        <v>0.4</v>
-      </c>
-      <c r="K30" s="21"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A31" s="156"/>
-      <c r="B31" s="155" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" s="47">
-        <v>1</v>
-      </c>
-      <c r="D31" s="49">
-        <v>0.7</v>
-      </c>
-      <c r="E31" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="97" t="s">
-        <v>230</v>
-      </c>
-      <c r="I31" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="J31" s="85">
-        <v>0.3</v>
-      </c>
+      <c r="I31" s="95"/>
+      <c r="J31" s="20"/>
       <c r="K31" s="21"/>
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" ht="28.5" customHeight="1">
       <c r="A32" s="156"/>
-      <c r="B32" s="157"/>
+      <c r="B32" s="48" t="s">
+        <v>159</v>
+      </c>
       <c r="C32" s="47">
         <v>1</v>
       </c>
@@ -3809,14 +3823,14 @@
       </c>
       <c r="F32" s="47"/>
       <c r="G32" s="47"/>
-      <c r="H32" s="97" t="s">
-        <v>231</v>
+      <c r="H32" s="96" t="s">
+        <v>108</v>
       </c>
       <c r="I32" s="52" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="J32" s="85">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="K32" s="21"/>
       <c r="L32" s="4"/>
@@ -3824,7 +3838,7 @@
     <row r="33" spans="1:12" ht="28.5" customHeight="1">
       <c r="A33" s="156"/>
       <c r="B33" s="155" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C33" s="47">
         <v>1</v>
@@ -3832,88 +3846,99 @@
       <c r="D33" s="49">
         <v>0.7</v>
       </c>
-      <c r="E33" s="161" t="s">
+      <c r="E33" s="50" t="s">
         <v>106</v>
       </c>
       <c r="F33" s="47"/>
       <c r="G33" s="47"/>
       <c r="H33" s="97" t="s">
-        <v>228</v>
-      </c>
-      <c r="I33" s="52"/>
-      <c r="J33" s="20"/>
+        <v>229</v>
+      </c>
+      <c r="I33" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" s="85">
+        <v>0.3</v>
+      </c>
       <c r="K33" s="21"/>
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" ht="28.5" customHeight="1">
       <c r="A34" s="156"/>
-      <c r="B34" s="156"/>
+      <c r="B34" s="157"/>
       <c r="C34" s="47">
         <v>1</v>
       </c>
       <c r="D34" s="49">
         <v>0.7</v>
       </c>
-      <c r="E34" s="162"/>
+      <c r="E34" s="50" t="s">
+        <v>106</v>
+      </c>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
       <c r="H34" s="97" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I34" s="52" t="s">
         <v>88</v>
       </c>
       <c r="J34" s="85">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="K34" s="21"/>
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" ht="28.5" customHeight="1">
       <c r="A35" s="156"/>
-      <c r="B35" s="157"/>
+      <c r="B35" s="155" t="s">
+        <v>161</v>
+      </c>
       <c r="C35" s="47">
         <v>1</v>
       </c>
       <c r="D35" s="49">
         <v>0.7</v>
       </c>
-      <c r="E35" s="135"/>
+      <c r="E35" s="158" t="s">
+        <v>106</v>
+      </c>
       <c r="F35" s="47"/>
       <c r="G35" s="47"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="J35" s="85">
-        <v>0.4</v>
-      </c>
+      <c r="H35" s="97" t="s">
+        <v>227</v>
+      </c>
+      <c r="I35" s="52"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="21"/>
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="28.5" customHeight="1">
       <c r="A36" s="156"/>
-      <c r="B36" s="155" t="s">
-        <v>160</v>
-      </c>
+      <c r="B36" s="156"/>
       <c r="C36" s="47">
         <v>1</v>
       </c>
       <c r="D36" s="49">
         <v>0.7</v>
       </c>
-      <c r="E36" s="161" t="s">
-        <v>106</v>
-      </c>
+      <c r="E36" s="159"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="H36" s="97" t="s">
-        <v>232</v>
-      </c>
-      <c r="I36" s="52"/>
+        <v>228</v>
+      </c>
+      <c r="I36" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="85">
+        <v>0.4</v>
+      </c>
+      <c r="K36" s="21"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A37" s="157"/>
+      <c r="A37" s="156"/>
       <c r="B37" s="157"/>
       <c r="C37" s="47">
         <v>1</v>
@@ -3921,18 +3946,23 @@
       <c r="D37" s="49">
         <v>0.7</v>
       </c>
-      <c r="E37" s="162"/>
+      <c r="E37" s="135"/>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
-      <c r="H37" s="97" t="s">
-        <v>233</v>
-      </c>
-      <c r="I37" s="52"/>
+      <c r="H37" s="97"/>
+      <c r="I37" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="J37" s="85">
+        <v>0.4</v>
+      </c>
+      <c r="K37" s="21"/>
+      <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A38" s="136"/>
-      <c r="B38" s="136" t="s">
-        <v>256</v>
+      <c r="A38" s="156"/>
+      <c r="B38" s="155" t="s">
+        <v>160</v>
       </c>
       <c r="C38" s="47">
         <v>1</v>
@@ -3940,57 +3970,93 @@
       <c r="D38" s="49">
         <v>0.7</v>
       </c>
-      <c r="E38" s="137"/>
+      <c r="E38" s="158" t="s">
+        <v>106</v>
+      </c>
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
       <c r="H38" s="97" t="s">
-        <v>257</v>
-      </c>
-      <c r="I38" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="J38" s="85">
+        <v>231</v>
+      </c>
+      <c r="I38" s="52"/>
+    </row>
+    <row r="39" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A39" s="156"/>
+      <c r="B39" s="157"/>
+      <c r="C39" s="47">
+        <v>1</v>
+      </c>
+      <c r="D39" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="E39" s="159"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="97" t="s">
+        <v>232</v>
+      </c>
+      <c r="I39" s="52"/>
+    </row>
+    <row r="40" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A40" s="157"/>
+      <c r="B40" s="136" t="s">
+        <v>255</v>
+      </c>
+      <c r="C40" s="47">
+        <v>1</v>
+      </c>
+      <c r="D40" s="49">
+        <v>0.7</v>
+      </c>
+      <c r="E40" s="137"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="97" t="s">
+        <v>299</v>
+      </c>
+      <c r="I40" s="52"/>
+      <c r="J40" s="85">
         <v>0.4</v>
       </c>
-      <c r="K38" s="21"/>
-      <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A39" s="98"/>
-      <c r="B39" s="86" t="s">
+      <c r="K40" s="21"/>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" ht="28.5" customHeight="1">
+      <c r="A41" s="98"/>
+      <c r="B41" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="86">
-        <v>1</v>
-      </c>
-      <c r="D39" s="87">
+      <c r="C41" s="86">
+        <v>1</v>
+      </c>
+      <c r="D41" s="87">
         <v>0.7</v>
       </c>
-      <c r="E39" s="50" t="s">
+      <c r="E41" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="F39" s="86"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A29:A37"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="E26:E28"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="A31:A40"/>
+    <mergeCell ref="A20:A30"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4003,30 +4069,31 @@
     <hyperlink ref="E10" r:id="rId7" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E11" r:id="rId8" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E13" r:id="rId9"/>
-    <hyperlink ref="E29" r:id="rId10"/>
+    <hyperlink ref="E31" r:id="rId10"/>
     <hyperlink ref="E14" r:id="rId11"/>
     <hyperlink ref="E12" r:id="rId12"/>
     <hyperlink ref="E16" r:id="rId13" location="files" display="http://www.thingiverse.com/thing:790533/ - files"/>
     <hyperlink ref="E18" r:id="rId14" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
     <hyperlink ref="E19" r:id="rId15" location="files" display="http://www.thingiverse.com/thing:902483/ - files"/>
-    <hyperlink ref="E30" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
+    <hyperlink ref="E32" r:id="rId16" display="http://www.thingiverse.com/thing:1234989"/>
     <hyperlink ref="E17" r:id="rId17"/>
-    <hyperlink ref="E31" r:id="rId18"/>
-    <hyperlink ref="E33" r:id="rId19"/>
+    <hyperlink ref="E33" r:id="rId18"/>
+    <hyperlink ref="E35" r:id="rId19"/>
     <hyperlink ref="E15" r:id="rId20" location="files" display="http://www.thingiverse.com/thing:729919/ - files"/>
-    <hyperlink ref="E36" r:id="rId21"/>
-    <hyperlink ref="E39" r:id="rId22"/>
+    <hyperlink ref="E38" r:id="rId21"/>
+    <hyperlink ref="E41" r:id="rId22"/>
     <hyperlink ref="E20" r:id="rId23"/>
     <hyperlink ref="E21" r:id="rId24"/>
     <hyperlink ref="E22" r:id="rId25"/>
-    <hyperlink ref="E32" r:id="rId26"/>
+    <hyperlink ref="E34" r:id="rId26"/>
     <hyperlink ref="E23" r:id="rId27"/>
     <hyperlink ref="E24" r:id="rId28"/>
     <hyperlink ref="E25" r:id="rId29"/>
     <hyperlink ref="E26" r:id="rId30"/>
+    <hyperlink ref="E29" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -4060,19 +4127,19 @@
         <v>21</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H1" s="116" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="116" t="s">
         <v>211</v>
-      </c>
-      <c r="I1" s="116" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4100,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4128,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4157,7 +4224,7 @@
         <v>8700</v>
       </c>
       <c r="I4" s="107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4185,7 +4252,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="107" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4269,10 +4336,10 @@
     </row>
     <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B9" s="110" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -4318,7 +4385,7 @@
         <v>46500</v>
       </c>
       <c r="I10" s="107" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4451,7 +4518,7 @@
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20" s="103"/>
       <c r="C20" s="9">
@@ -4464,7 +4531,7 @@
       </c>
       <c r="H20" s="104"/>
       <c r="I20" s="118" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4472,16 +4539,16 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="102" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G22" s="105"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="101" t="s">
         <v>195</v>
-      </c>
-      <c r="B23" s="101" t="s">
-        <v>196</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
@@ -4508,16 +4575,16 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="102" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G25" s="105"/>
     </row>
     <row r="26" spans="1:9" ht="28.5">
       <c r="A26" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B26" s="101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -4544,16 +4611,16 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="102" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G28" s="105"/>
     </row>
     <row r="29" spans="1:9" ht="28.5">
       <c r="A29" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29" s="101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" s="9">
         <v>1</v>
@@ -4587,7 +4654,7 @@
     </row>
     <row r="32" spans="1:9" ht="26.25">
       <c r="D32" s="131" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E32" s="132">
         <f>E17+E30</f>
@@ -4631,8 +4698,8 @@
   </sheetPr>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4670,19 +4737,19 @@
         <v>21</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>69</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K1" s="44"/>
     </row>
@@ -4738,7 +4805,7 @@
       <c r="C3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="168" t="s">
+      <c r="D3" s="178" t="s">
         <v>143</v>
       </c>
       <c r="E3" s="34">
@@ -4762,7 +4829,7 @@
         <v>88</v>
       </c>
       <c r="K3" s="43"/>
-      <c r="L3" s="166" t="s">
+      <c r="L3" s="176" t="s">
         <v>98</v>
       </c>
       <c r="M3" s="19" t="s">
@@ -4784,7 +4851,7 @@
       <c r="C4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="179"/>
       <c r="E4" s="6">
         <v>8</v>
       </c>
@@ -4806,7 +4873,7 @@
         <v>88</v>
       </c>
       <c r="K4" s="43"/>
-      <c r="L4" s="167"/>
+      <c r="L4" s="177"/>
       <c r="M4" s="19" t="s">
         <v>91</v>
       </c>
@@ -4826,7 +4893,7 @@
       <c r="C5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="179"/>
       <c r="E5" s="6">
         <v>2</v>
       </c>
@@ -4848,7 +4915,7 @@
         <v>88</v>
       </c>
       <c r="K5" s="43"/>
-      <c r="L5" s="167"/>
+      <c r="L5" s="177"/>
       <c r="M5" s="19" t="s">
         <v>92</v>
       </c>
@@ -4868,7 +4935,7 @@
       <c r="C6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="179"/>
       <c r="E6" s="6">
         <v>2</v>
       </c>
@@ -4903,7 +4970,7 @@
       <c r="C7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="170"/>
+      <c r="D7" s="180"/>
       <c r="E7" s="7">
         <v>28</v>
       </c>
@@ -4926,7 +4993,7 @@
         <v>88</v>
       </c>
       <c r="K7" s="43"/>
-      <c r="L7" s="166" t="s">
+      <c r="L7" s="176" t="s">
         <v>99</v>
       </c>
       <c r="M7" s="19" t="s">
@@ -4982,7 +5049,7 @@
         <v>88</v>
       </c>
       <c r="K8" s="43"/>
-      <c r="L8" s="166"/>
+      <c r="L8" s="176"/>
       <c r="M8" s="19" t="s">
         <v>96</v>
       </c>
@@ -5034,7 +5101,7 @@
         <v>88</v>
       </c>
       <c r="K9" s="43"/>
-      <c r="L9" s="166"/>
+      <c r="L9" s="176"/>
       <c r="M9" s="19" t="s">
         <v>97</v>
       </c>
@@ -5064,7 +5131,7 @@
       <c r="C10" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="168" t="s">
+      <c r="D10" s="178" t="s">
         <v>140</v>
       </c>
       <c r="E10" s="34">
@@ -5090,7 +5157,7 @@
       </c>
       <c r="K10" s="43"/>
       <c r="M10" s="82" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N10">
         <v>25</v>
@@ -5111,7 +5178,7 @@
       <c r="C11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="169"/>
+      <c r="D11" s="179"/>
       <c r="E11" s="6">
         <v>3</v>
       </c>
@@ -5146,7 +5213,7 @@
       <c r="C12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="170"/>
+      <c r="D12" s="180"/>
       <c r="E12" s="7">
         <v>36</v>
       </c>
@@ -5193,7 +5260,7 @@
       <c r="C13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="168" t="s">
+      <c r="D13" s="178" t="s">
         <v>142</v>
       </c>
       <c r="E13" s="34">
@@ -5226,7 +5293,7 @@
       <c r="C14" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="169"/>
+      <c r="D14" s="179"/>
       <c r="E14" s="6">
         <v>34</v>
       </c>
@@ -5249,13 +5316,13 @@
       </c>
       <c r="K14" s="43"/>
       <c r="N14" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="O14" s="105" t="s">
         <v>279</v>
       </c>
-      <c r="O14" s="105" t="s">
-        <v>281</v>
-      </c>
       <c r="P14" s="105" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q14" s="105"/>
     </row>
@@ -5267,7 +5334,7 @@
       <c r="C15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="170"/>
+      <c r="D15" s="180"/>
       <c r="E15" s="7">
         <v>22</v>
       </c>
@@ -5290,7 +5357,7 @@
       </c>
       <c r="K15" s="43"/>
       <c r="L15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N15">
         <f>42-15</f>
@@ -5320,7 +5387,7 @@
       <c r="J16" s="30"/>
       <c r="K16" s="43"/>
       <c r="L16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N16">
         <f>(N7*10)-(N15*2)</f>
@@ -5359,7 +5426,7 @@
       <c r="J17" s="31"/>
       <c r="K17" s="43"/>
       <c r="L17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="O17">
         <v>13</v>
@@ -5374,16 +5441,16 @@
     </row>
     <row r="18" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="109" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="103" t="s">
         <v>206</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D18" s="103" t="s">
-        <v>207</v>
       </c>
       <c r="E18" s="9">
         <v>4</v>
@@ -5400,7 +5467,7 @@
         <v>5423.9999999999991</v>
       </c>
       <c r="I18" s="104">
-        <f>E18*H18</f>
+        <f t="shared" ref="I18:I23" si="4">E18*H18</f>
         <v>21695.999999999996</v>
       </c>
       <c r="J18" s="106" t="s">
@@ -5414,16 +5481,16 @@
     </row>
     <row r="19" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="109" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="103" t="s">
         <v>239</v>
-      </c>
-      <c r="D19" s="103" t="s">
-        <v>240</v>
       </c>
       <c r="E19" s="9">
         <v>1</v>
@@ -5436,7 +5503,7 @@
         <v>9900</v>
       </c>
       <c r="I19" s="104">
-        <f>E19*H19</f>
+        <f t="shared" si="4"/>
         <v>9900</v>
       </c>
       <c r="J19" s="134" t="s">
@@ -5446,16 +5513,16 @@
     </row>
     <row r="20" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="109" t="s">
+        <v>240</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="103" t="s">
         <v>242</v>
-      </c>
-      <c r="D20" s="103" t="s">
-        <v>243</v>
       </c>
       <c r="E20" s="9">
         <v>1</v>
@@ -5468,7 +5535,7 @@
         <v>19900</v>
       </c>
       <c r="I20" s="104">
-        <f>E20*H20</f>
+        <f t="shared" si="4"/>
         <v>19900</v>
       </c>
       <c r="J20" s="134" t="s">
@@ -5478,14 +5545,14 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="171" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="183" t="s">
-        <v>286</v>
+      <c r="D21" s="168" t="s">
+        <v>284</v>
       </c>
       <c r="E21" s="9">
         <v>4</v>
@@ -5496,7 +5563,7 @@
         <v>3710</v>
       </c>
       <c r="I21" s="104">
-        <f>E21*H21</f>
+        <f t="shared" si="4"/>
         <v>14840</v>
       </c>
       <c r="J21" s="138"/>
@@ -5505,10 +5572,10 @@
     <row r="22" spans="1:17">
       <c r="A22" s="172"/>
       <c r="B22" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="184"/>
+      <c r="D22" s="169"/>
       <c r="E22" s="9">
         <v>4</v>
       </c>
@@ -5518,7 +5585,7 @@
         <v>1710</v>
       </c>
       <c r="I22" s="104">
-        <f>E22*H22</f>
+        <f t="shared" si="4"/>
         <v>6840</v>
       </c>
       <c r="J22" s="138"/>
@@ -5527,10 +5594,10 @@
     <row r="23" spans="1:17">
       <c r="A23" s="173"/>
       <c r="B23" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="185"/>
+      <c r="D23" s="170"/>
       <c r="E23" s="9">
         <v>12</v>
       </c>
@@ -5540,7 +5607,7 @@
         <v>500</v>
       </c>
       <c r="I23" s="104">
-        <f>E23*H23</f>
+        <f t="shared" si="4"/>
         <v>6000</v>
       </c>
       <c r="J23" s="138"/>
@@ -5548,16 +5615,16 @@
     </row>
     <row r="24" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="109" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>294</v>
-      </c>
       <c r="D24" s="103" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="138"/>
@@ -5570,11 +5637,11 @@
       <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:17">
-      <c r="B26" s="182"/>
+      <c r="B26" s="150"/>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:17">
-      <c r="B27" s="186"/>
+      <c r="B27" s="151"/>
     </row>
     <row r="28" spans="1:17">
       <c r="B28" s="41"/>
@@ -5601,7 +5668,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4"/>
-      <c r="B33" s="182"/>
+      <c r="B33" s="150"/>
     </row>
     <row r="34" spans="1:2">
       <c r="B34" s="22"/>
@@ -5609,6 +5676,11 @@
     <row r="49" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A3:A7"/>
@@ -5616,11 +5688,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5688,7 +5755,7 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="181" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="72" t="s">
@@ -5697,10 +5764,10 @@
       <c r="C2" s="29">
         <v>4</v>
       </c>
-      <c r="D2" s="178">
+      <c r="D2" s="183">
         <v>4</v>
       </c>
-      <c r="E2" s="178">
+      <c r="E2" s="183">
         <v>6</v>
       </c>
       <c r="H2" s="143">
@@ -5753,35 +5820,35 @@
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="177"/>
+      <c r="A3" s="182"/>
       <c r="B3" s="72" t="s">
         <v>164</v>
       </c>
       <c r="C3" s="29">
         <v>2</v>
       </c>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
       <c r="H3" s="143" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="143" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="143" t="s">
         <v>258</v>
       </c>
-      <c r="I3" s="143" t="s">
+      <c r="K3" s="143" t="s">
         <v>259</v>
       </c>
-      <c r="J3" s="143" t="s">
+      <c r="L3" s="143" t="s">
         <v>260</v>
       </c>
-      <c r="K3" s="143" t="s">
-        <v>261</v>
-      </c>
-      <c r="L3" s="143" t="s">
-        <v>262</v>
-      </c>
       <c r="M3" s="143" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N3" s="143" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O3" s="79"/>
       <c r="P3" s="79"/>
@@ -5796,7 +5863,7 @@
         <v>182</v>
       </c>
       <c r="V3" s="144" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="W3" s="148"/>
       <c r="X3" s="149" t="s">
@@ -5804,131 +5871,131 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="177"/>
+      <c r="A4" s="182"/>
       <c r="B4" s="83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="179"/>
-      <c r="E4" s="179"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="184"/>
       <c r="H4" s="139" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" s="139" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="139" t="s">
         <v>263</v>
       </c>
-      <c r="I4" s="139" t="s">
+      <c r="K4" s="139" t="s">
         <v>264</v>
       </c>
-      <c r="J4" s="139" t="s">
+      <c r="L4" s="139" t="s">
         <v>265</v>
       </c>
-      <c r="K4" s="139" t="s">
+      <c r="M4" s="139" t="s">
         <v>266</v>
       </c>
-      <c r="L4" s="139" t="s">
+      <c r="N4" s="139" t="s">
         <v>267</v>
-      </c>
-      <c r="M4" s="139" t="s">
-        <v>268</v>
-      </c>
-      <c r="N4" s="139" t="s">
-        <v>269</v>
       </c>
       <c r="O4" s="82"/>
       <c r="P4" s="105"/>
       <c r="Q4" s="105"/>
       <c r="R4" s="105"/>
       <c r="S4" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="T4" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="U4" s="140" t="s">
         <v>270</v>
       </c>
-      <c r="T4" s="140" t="s">
-        <v>271</v>
-      </c>
-      <c r="U4" s="140" t="s">
+      <c r="V4" s="141" t="s">
         <v>272</v>
-      </c>
-      <c r="V4" s="141" t="s">
-        <v>274</v>
       </c>
       <c r="W4" s="105"/>
       <c r="X4" s="140" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="182"/>
+      <c r="B5" s="84" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="29">
+        <v>1</v>
+      </c>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
+      <c r="N5" s="142" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="182"/>
+      <c r="B6" s="81" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="70">
+        <v>1</v>
+      </c>
+      <c r="D6" s="184"/>
+      <c r="E6" s="184"/>
+      <c r="H6" s="139" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
-      <c r="A5" s="177"/>
-      <c r="B5" s="84" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="29">
-        <v>1</v>
-      </c>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
-      <c r="N5" s="142" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="A6" s="177"/>
-      <c r="B6" s="81" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" s="70">
-        <v>1</v>
-      </c>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="H6" s="139" t="s">
-        <v>275</v>
-      </c>
       <c r="I6" s="140" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="177"/>
+      <c r="A7" s="182"/>
       <c r="B7" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C7" s="70">
         <v>1</v>
       </c>
-      <c r="D7" s="179"/>
-      <c r="E7" s="179"/>
+      <c r="D7" s="184"/>
+      <c r="E7" s="184"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="181" t="s">
         <v>166</v>
       </c>
       <c r="B8" s="83" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C8" s="71">
         <v>1</v>
       </c>
-      <c r="D8" s="178">
+      <c r="D8" s="183">
         <v>2</v>
       </c>
-      <c r="E8" s="178">
+      <c r="E8" s="183">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="177"/>
+      <c r="A9" s="182"/>
       <c r="B9" s="74" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="71">
         <v>1</v>
       </c>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
       <c r="H9" t="s">
+        <v>221</v>
+      </c>
+      <c r="J9" t="s">
         <v>222</v>
-      </c>
-      <c r="J9" t="s">
-        <v>223</v>
       </c>
       <c r="K9" s="80">
         <v>290</v>
@@ -5941,19 +6008,19 @@
         <v>1450</v>
       </c>
       <c r="P9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="181"/>
+      <c r="A10" s="186"/>
       <c r="B10" s="75" t="s">
         <v>167</v>
       </c>
       <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
       <c r="H10" t="s">
         <v>178</v>
       </c>
@@ -5971,12 +6038,12 @@
         <v>1950</v>
       </c>
       <c r="P10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:24">
       <c r="H11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K11" s="80">
         <v>50</v>
@@ -6009,7 +6076,7 @@
         <v>179</v>
       </c>
       <c r="J13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K13" s="80">
         <v>510</v>
@@ -6022,7 +6089,7 @@
         <v>2550</v>
       </c>
       <c r="P13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -6043,7 +6110,7 @@
         <v>1050</v>
       </c>
       <c r="P14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:24">

</xml_diff>

<commit_message>
z working area reduced
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\03.Mostly-Printed-CNC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\Mostly-Printed-CNC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="306">
   <si>
     <t>QTY</t>
   </si>
@@ -1158,22 +1158,58 @@
     </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>working
+area</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conduit
+length</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>leg</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thread</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>belt</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="179" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="167" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
   </numFmts>
   <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1202,14 +1238,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1230,7 +1266,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1239,7 +1275,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1248,7 +1284,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1286,14 +1322,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1308,7 +1344,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1316,7 +1352,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1324,7 +1360,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1332,7 +1368,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1340,14 +1376,14 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1618,7 +1654,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1658,19 +1694,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1682,7 +1718,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -1730,7 +1766,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1739,7 +1775,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1823,7 +1859,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1859,7 +1895,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1931,7 +1967,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1970,10 +2006,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1982,22 +2018,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2015,10 +2051,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2069,6 +2105,48 @@
     <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2084,37 +2162,28 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2132,21 +2201,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2165,25 +2219,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2213,8 +2270,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>399501</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>199476</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>15850</xdr:rowOff>
     </xdr:to>
@@ -2695,7 +2752,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2963,16 +3020,16 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="45.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="4" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="41.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3010,7 +3067,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="150" t="s">
+      <c r="A4" s="164" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="69" t="s">
@@ -3042,7 +3099,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="151"/>
+      <c r="A5" s="165"/>
       <c r="B5" s="48" t="s">
         <v>77</v>
       </c>
@@ -3072,7 +3129,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="166" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="53" t="s">
@@ -3104,7 +3161,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A7" s="153"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="53" t="s">
         <v>7</v>
       </c>
@@ -3134,7 +3191,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A8" s="154"/>
+      <c r="A8" s="168"/>
       <c r="B8" s="53" t="s">
         <v>8</v>
       </c>
@@ -3164,7 +3221,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A9" s="155" t="s">
+      <c r="A9" s="156" t="s">
         <v>154</v>
       </c>
       <c r="B9" s="48" t="s">
@@ -3196,7 +3253,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A10" s="156"/>
+      <c r="A10" s="157"/>
       <c r="B10" s="48" t="s">
         <v>10</v>
       </c>
@@ -3226,7 +3283,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A11" s="156"/>
+      <c r="A11" s="157"/>
       <c r="B11" s="48" t="s">
         <v>11</v>
       </c>
@@ -3256,7 +3313,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A12" s="157"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
@@ -3286,7 +3343,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A13" s="152" t="s">
+      <c r="A13" s="166" t="s">
         <v>155</v>
       </c>
       <c r="B13" s="53" t="s">
@@ -3318,7 +3375,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A14" s="153"/>
+      <c r="A14" s="167"/>
       <c r="B14" s="53" t="s">
         <v>16</v>
       </c>
@@ -3348,7 +3405,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A15" s="153"/>
+      <c r="A15" s="167"/>
       <c r="B15" s="53" t="s">
         <v>123</v>
       </c>
@@ -3378,7 +3435,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A16" s="153"/>
+      <c r="A16" s="167"/>
       <c r="B16" s="60" t="s">
         <v>19</v>
       </c>
@@ -3403,7 +3460,7 @@
       <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A17" s="154"/>
+      <c r="A17" s="168"/>
       <c r="B17" s="53" t="s">
         <v>119</v>
       </c>
@@ -3424,7 +3481,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A18" s="155" t="s">
+      <c r="A18" s="156" t="s">
         <v>156</v>
       </c>
       <c r="B18" s="48" t="s">
@@ -3456,7 +3513,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A19" s="157"/>
+      <c r="A19" s="158"/>
       <c r="B19" s="48" t="s">
         <v>74</v>
       </c>
@@ -3486,7 +3543,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A20" s="158" t="s">
+      <c r="A20" s="153" t="s">
         <v>149</v>
       </c>
       <c r="B20" s="88" t="s">
@@ -3514,7 +3571,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A21" s="159"/>
+      <c r="A21" s="154"/>
       <c r="B21" s="88" t="s">
         <v>191</v>
       </c>
@@ -3540,8 +3597,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A22" s="159"/>
-      <c r="B22" s="158" t="s">
+      <c r="A22" s="154"/>
+      <c r="B22" s="153" t="s">
         <v>194</v>
       </c>
       <c r="C22" s="88">
@@ -3566,8 +3623,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A23" s="159"/>
-      <c r="B23" s="159"/>
+      <c r="A23" s="154"/>
+      <c r="B23" s="154"/>
       <c r="C23" s="88">
         <v>1</v>
       </c>
@@ -3590,8 +3647,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A24" s="159"/>
-      <c r="B24" s="160"/>
+      <c r="A24" s="154"/>
+      <c r="B24" s="155"/>
       <c r="C24" s="88">
         <v>1</v>
       </c>
@@ -3614,7 +3671,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A25" s="159"/>
+      <c r="A25" s="154"/>
       <c r="B25" s="88" t="s">
         <v>250</v>
       </c>
@@ -3640,8 +3697,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A26" s="159"/>
-      <c r="B26" s="158" t="s">
+      <c r="A26" s="154"/>
+      <c r="B26" s="153" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="88">
@@ -3650,7 +3707,7 @@
       <c r="D26" s="89">
         <v>0.5</v>
       </c>
-      <c r="E26" s="163" t="s">
+      <c r="E26" s="161" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="88"/>
@@ -3666,15 +3723,15 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A27" s="159"/>
-      <c r="B27" s="159"/>
+      <c r="A27" s="154"/>
+      <c r="B27" s="154"/>
       <c r="C27" s="88">
         <v>1</v>
       </c>
       <c r="D27" s="89">
         <v>0.5</v>
       </c>
-      <c r="E27" s="164"/>
+      <c r="E27" s="162"/>
       <c r="F27" s="88"/>
       <c r="G27" s="57"/>
       <c r="H27" s="100" t="s">
@@ -3688,15 +3745,15 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A28" s="160"/>
-      <c r="B28" s="160"/>
+      <c r="A28" s="155"/>
+      <c r="B28" s="155"/>
       <c r="C28" s="88">
         <v>1</v>
       </c>
       <c r="D28" s="89">
         <v>0.5</v>
       </c>
-      <c r="E28" s="165"/>
+      <c r="E28" s="163"/>
       <c r="F28" s="88"/>
       <c r="G28" s="57"/>
       <c r="H28" s="100" t="s">
@@ -3710,7 +3767,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A29" s="155" t="s">
+      <c r="A29" s="156" t="s">
         <v>162</v>
       </c>
       <c r="B29" s="90" t="s">
@@ -3740,7 +3797,7 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A30" s="156"/>
+      <c r="A30" s="157"/>
       <c r="B30" s="48" t="s">
         <v>159</v>
       </c>
@@ -3768,8 +3825,8 @@
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A31" s="156"/>
-      <c r="B31" s="155" t="s">
+      <c r="A31" s="157"/>
+      <c r="B31" s="156" t="s">
         <v>158</v>
       </c>
       <c r="C31" s="47">
@@ -3796,8 +3853,8 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A32" s="156"/>
-      <c r="B32" s="157"/>
+      <c r="A32" s="157"/>
+      <c r="B32" s="158"/>
       <c r="C32" s="47">
         <v>1</v>
       </c>
@@ -3822,8 +3879,8 @@
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A33" s="156"/>
-      <c r="B33" s="155" t="s">
+      <c r="A33" s="157"/>
+      <c r="B33" s="156" t="s">
         <v>161</v>
       </c>
       <c r="C33" s="47">
@@ -3832,7 +3889,7 @@
       <c r="D33" s="49">
         <v>0.7</v>
       </c>
-      <c r="E33" s="161" t="s">
+      <c r="E33" s="159" t="s">
         <v>106</v>
       </c>
       <c r="F33" s="47"/>
@@ -3846,15 +3903,15 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A34" s="156"/>
-      <c r="B34" s="156"/>
+      <c r="A34" s="157"/>
+      <c r="B34" s="157"/>
       <c r="C34" s="47">
         <v>1</v>
       </c>
       <c r="D34" s="49">
         <v>0.7</v>
       </c>
-      <c r="E34" s="162"/>
+      <c r="E34" s="160"/>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
       <c r="H34" s="97" t="s">
@@ -3870,8 +3927,8 @@
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A35" s="156"/>
-      <c r="B35" s="157"/>
+      <c r="A35" s="157"/>
+      <c r="B35" s="158"/>
       <c r="C35" s="47">
         <v>1</v>
       </c>
@@ -3892,8 +3949,8 @@
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A36" s="156"/>
-      <c r="B36" s="155" t="s">
+      <c r="A36" s="157"/>
+      <c r="B36" s="156" t="s">
         <v>160</v>
       </c>
       <c r="C36" s="47">
@@ -3902,7 +3959,7 @@
       <c r="D36" s="49">
         <v>0.7</v>
       </c>
-      <c r="E36" s="161" t="s">
+      <c r="E36" s="159" t="s">
         <v>106</v>
       </c>
       <c r="F36" s="47"/>
@@ -3913,15 +3970,15 @@
       <c r="I36" s="52"/>
     </row>
     <row r="37" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A37" s="157"/>
-      <c r="B37" s="157"/>
+      <c r="A37" s="158"/>
+      <c r="B37" s="158"/>
       <c r="C37" s="47">
         <v>1</v>
       </c>
       <c r="D37" s="49">
         <v>0.7</v>
       </c>
-      <c r="E37" s="162"/>
+      <c r="E37" s="160"/>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
       <c r="H37" s="97" t="s">
@@ -3976,6 +4033,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A13:A17"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="A29:A37"/>
     <mergeCell ref="E33:E34"/>
@@ -3986,11 +4048,6 @@
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="E26:E28"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4038,15 +4095,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4585,7 +4642,7 @@
         <v>31536</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="26.25">
+    <row r="32" spans="1:9" ht="21">
       <c r="D32" s="131" t="s">
         <v>217</v>
       </c>
@@ -4629,31 +4686,36 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="107.625" customWidth="1"/>
-    <col min="5" max="5" width="8.125" customWidth="1"/>
-    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="107.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.375" customWidth="1"/>
-    <col min="14" max="14" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="16" max="16" width="5.5703125" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>144</v>
       </c>
@@ -4685,8 +4747,11 @@
         <v>209</v>
       </c>
       <c r="K1" s="44"/>
-    </row>
-    <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1">
+      <c r="P1" s="105" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="46" t="s">
         <v>150</v>
       </c>
@@ -4720,16 +4785,21 @@
       </c>
       <c r="K2" s="43"/>
       <c r="L2" s="23"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19" t="s">
+      <c r="M2" s="150"/>
+      <c r="N2" s="189" t="s">
+        <v>296</v>
+      </c>
+      <c r="U2" s="23"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="X2" s="19" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="171" t="s">
+    <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="172" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="34" t="s">
@@ -4738,7 +4808,7 @@
       <c r="C3" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="168" t="s">
+      <c r="D3" s="179" t="s">
         <v>143</v>
       </c>
       <c r="E3" s="34">
@@ -4762,29 +4832,38 @@
         <v>88</v>
       </c>
       <c r="K3" s="43"/>
-      <c r="L3" s="166" t="s">
+      <c r="L3" s="177" t="s">
+        <v>297</v>
+      </c>
+      <c r="M3" s="150" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3" s="23">
+        <v>400</v>
+      </c>
+      <c r="U3" s="177" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="V3" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="23">
+      <c r="W3" s="23">
         <v>40</v>
       </c>
-      <c r="O3" s="23">
-        <f>N3/2.54</f>
+      <c r="X3" s="23">
+        <f>W3/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="172"/>
+    <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="173"/>
       <c r="B4" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="169"/>
+      <c r="D4" s="180"/>
       <c r="E4" s="6">
         <v>8</v>
       </c>
@@ -4806,27 +4885,34 @@
         <v>88</v>
       </c>
       <c r="K4" s="43"/>
-      <c r="L4" s="167"/>
-      <c r="M4" s="19" t="s">
+      <c r="L4" s="178"/>
+      <c r="M4" s="150" t="s">
         <v>91</v>
       </c>
       <c r="N4" s="23">
+        <v>400</v>
+      </c>
+      <c r="U4" s="178"/>
+      <c r="V4" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="W4" s="23">
         <v>40</v>
       </c>
-      <c r="O4" s="23">
-        <f t="shared" ref="O4:O5" si="2">N4/2.54</f>
+      <c r="X4" s="23">
+        <f t="shared" ref="X4:X5" si="2">W4/2.54</f>
         <v>15.748031496062993</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="172"/>
+    <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="173"/>
       <c r="B5" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="169"/>
+      <c r="D5" s="180"/>
       <c r="E5" s="6">
         <v>2</v>
       </c>
@@ -4848,27 +4934,34 @@
         <v>88</v>
       </c>
       <c r="K5" s="43"/>
-      <c r="L5" s="167"/>
-      <c r="M5" s="19" t="s">
+      <c r="L5" s="178"/>
+      <c r="M5" s="150" t="s">
         <v>92</v>
       </c>
       <c r="N5" s="23">
+        <v>150</v>
+      </c>
+      <c r="U5" s="178"/>
+      <c r="V5" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="W5" s="23">
         <v>25</v>
       </c>
-      <c r="O5" s="23">
+      <c r="X5" s="23">
         <f t="shared" si="2"/>
         <v>9.8425196850393704</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="172"/>
+    <row r="6" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="173"/>
       <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="169"/>
+      <c r="D6" s="180"/>
       <c r="E6" s="6">
         <v>2</v>
       </c>
@@ -4893,17 +4986,20 @@
       <c r="L6" s="24"/>
       <c r="M6" s="24"/>
       <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-    </row>
-    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="173"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+    </row>
+    <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="174"/>
       <c r="B7" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="170"/>
+      <c r="D7" s="181"/>
       <c r="E7" s="7">
         <v>28</v>
       </c>
@@ -4926,30 +5022,47 @@
         <v>88</v>
       </c>
       <c r="K7" s="43"/>
-      <c r="L7" s="166" t="s">
-        <v>99</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" s="23">
-        <f>N3+27</f>
-        <v>67</v>
-      </c>
-      <c r="O7" s="23">
-        <f>N7/2.54</f>
-        <v>26.377952755905511</v>
+      <c r="L7" s="177" t="s">
+        <v>298</v>
+      </c>
+      <c r="M7" s="150" t="s">
+        <v>90</v>
+      </c>
+      <c r="N7" s="193">
+        <f>N3+264</f>
+        <v>664</v>
       </c>
       <c r="P7">
         <v>3</v>
       </c>
       <c r="Q7">
         <f>N7*P7</f>
+        <v>1992</v>
+      </c>
+      <c r="U7" s="190" t="s">
+        <v>99</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="W7" s="23">
+        <f>W3+27</f>
+        <v>67</v>
+      </c>
+      <c r="X7" s="23">
+        <f>W7/2.54</f>
+        <v>26.377952755905511</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7">
+        <f>W7*Y7</f>
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="174" t="s">
+    <row r="8" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="175" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="35" t="s">
@@ -4982,28 +5095,43 @@
         <v>88</v>
       </c>
       <c r="K8" s="43"/>
-      <c r="L8" s="166"/>
-      <c r="M8" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="N8" s="23">
-        <f>N4+27</f>
-        <v>67</v>
-      </c>
-      <c r="O8" s="23">
-        <f>N8/2.54</f>
-        <v>26.377952755905511</v>
+      <c r="L8" s="177"/>
+      <c r="M8" s="150" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="193">
+        <f>N4+264</f>
+        <v>664</v>
       </c>
       <c r="P8">
         <v>3</v>
       </c>
       <c r="Q8">
         <f>N8*P8</f>
+        <v>1992</v>
+      </c>
+      <c r="U8" s="191"/>
+      <c r="V8" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="W8" s="23">
+        <f>W4+27</f>
+        <v>67</v>
+      </c>
+      <c r="X8" s="23">
+        <f>W8/2.54</f>
+        <v>26.377952755905511</v>
+      </c>
+      <c r="Y8">
+        <v>3</v>
+      </c>
+      <c r="Z8">
+        <f>W8*Y8</f>
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="175"/>
+    <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="176"/>
       <c r="B9" s="38" t="s">
         <v>139</v>
       </c>
@@ -5034,28 +5162,47 @@
         <v>88</v>
       </c>
       <c r="K9" s="43"/>
-      <c r="L9" s="166"/>
-      <c r="M9" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="N9" s="23">
-        <f>N5+20</f>
-        <v>45</v>
-      </c>
-      <c r="O9" s="23">
-        <f>N9/2.54</f>
-        <v>17.716535433070867</v>
+      <c r="L9" s="177"/>
+      <c r="M9" s="150" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="193">
+        <f>N5+190</f>
+        <v>340</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
       <c r="Q9">
         <f>N9*P9</f>
+        <v>680</v>
+      </c>
+      <c r="S9">
+        <f>W9*10-N9</f>
+        <v>110</v>
+      </c>
+      <c r="U9" s="191"/>
+      <c r="V9" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="W9" s="23">
+        <f>W5+20</f>
+        <v>45</v>
+      </c>
+      <c r="X9" s="23">
+        <f>W9/2.54</f>
+        <v>17.716535433070867</v>
+      </c>
+      <c r="Y9">
+        <v>2</v>
+      </c>
+      <c r="Z9">
+        <f>W9*Y9</f>
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="171" t="s">
+    <row r="10" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="172" t="s">
         <v>147</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -5064,7 +5211,7 @@
       <c r="C10" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="168" t="s">
+      <c r="D10" s="179" t="s">
         <v>140</v>
       </c>
       <c r="E10" s="34">
@@ -5089,29 +5236,50 @@
         <v>88</v>
       </c>
       <c r="K10" s="43"/>
-      <c r="M10" s="82" t="s">
-        <v>283</v>
-      </c>
-      <c r="N10">
-        <v>25</v>
+      <c r="L10" s="177"/>
+      <c r="M10" s="150" t="s">
+        <v>299</v>
+      </c>
+      <c r="N10" s="193">
+        <f>N5-13</f>
+        <v>137</v>
       </c>
       <c r="P10">
         <v>4</v>
       </c>
       <c r="Q10">
         <f>N10*P10</f>
+        <v>548</v>
+      </c>
+      <c r="S10">
+        <f>W10*10-N10</f>
+        <v>113</v>
+      </c>
+      <c r="U10" s="192"/>
+      <c r="V10" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="W10" s="23">
+        <v>25</v>
+      </c>
+      <c r="X10" s="23"/>
+      <c r="Y10">
+        <v>4</v>
+      </c>
+      <c r="Z10">
+        <f>W10*Y10</f>
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="172"/>
+    <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="173"/>
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="169"/>
+      <c r="D11" s="180"/>
       <c r="E11" s="6">
         <v>3</v>
       </c>
@@ -5135,18 +5303,22 @@
       <c r="K11" s="43"/>
       <c r="Q11">
         <f>SUM(Q7:Q10)</f>
+        <v>5212</v>
+      </c>
+      <c r="Z11">
+        <f>SUM(Z7:Z10)</f>
         <v>592</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="173"/>
+    <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="174"/>
       <c r="B12" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="170"/>
+      <c r="D12" s="181"/>
       <c r="E12" s="7">
         <v>36</v>
       </c>
@@ -5168,23 +5340,41 @@
         <v>88</v>
       </c>
       <c r="K12" s="43"/>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="150" t="s">
+        <v>300</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" s="193">
+        <f>N5+76</f>
+        <v>226</v>
+      </c>
+      <c r="O12" s="188" t="s">
+        <v>305</v>
+      </c>
+      <c r="P12" s="4"/>
+      <c r="S12">
+        <f>W12*10-N12</f>
+        <v>173.20000000000005</v>
+      </c>
+      <c r="U12" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="25" t="s">
+      <c r="V12" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="23">
-        <f>2.54*O12</f>
+      <c r="W12" s="23">
+        <f>2.54*X12</f>
         <v>39.92</v>
       </c>
-      <c r="O12" s="23">
-        <f>O9-2</f>
+      <c r="X12" s="23">
+        <f>X9-2</f>
         <v>15.716535433070867</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="171" t="s">
+    <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="172" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="34" t="s">
@@ -5193,7 +5383,7 @@
       <c r="C13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="168" t="s">
+      <c r="D13" s="179" t="s">
         <v>142</v>
       </c>
       <c r="E13" s="34">
@@ -5217,16 +5407,18 @@
         <v>88</v>
       </c>
       <c r="K13" s="43"/>
-    </row>
-    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="172"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+    </row>
+    <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="173"/>
       <c r="B14" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="169"/>
+      <c r="D14" s="180"/>
       <c r="E14" s="6">
         <v>34</v>
       </c>
@@ -5248,26 +5440,42 @@
         <v>88</v>
       </c>
       <c r="K14" s="43"/>
-      <c r="N14" s="105" t="s">
+      <c r="L14" s="182" t="s">
+        <v>301</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="N14" s="23">
+        <f>N3+400</f>
+        <v>800</v>
+      </c>
+      <c r="O14" t="s">
+        <v>305</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="W14" s="105" t="s">
         <v>279</v>
       </c>
-      <c r="O14" s="105" t="s">
+      <c r="X14" s="105" t="s">
         <v>281</v>
       </c>
-      <c r="P14" s="105" t="s">
+      <c r="Y14" s="105" t="s">
         <v>282</v>
       </c>
-      <c r="Q14" s="105"/>
-    </row>
-    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="173"/>
+      <c r="Z14" s="105"/>
+    </row>
+    <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="174"/>
       <c r="B15" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="170"/>
+      <c r="D15" s="181"/>
       <c r="E15" s="7">
         <v>22</v>
       </c>
@@ -5289,16 +5497,30 @@
         <v>88</v>
       </c>
       <c r="K15" s="43"/>
-      <c r="L15" t="s">
+      <c r="L15" s="187"/>
+      <c r="M15" s="150" t="s">
+        <v>303</v>
+      </c>
+      <c r="N15" s="23">
+        <f>N4+400</f>
+        <v>800</v>
+      </c>
+      <c r="O15" t="s">
+        <v>305</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="U15" t="s">
         <v>278</v>
       </c>
-      <c r="N15">
+      <c r="W15">
         <f>42-15</f>
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="171" t="s">
+    <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="172" t="s">
         <v>149</v>
       </c>
       <c r="B16" s="34" t="s">
@@ -5319,27 +5541,29 @@
       <c r="I16" s="14"/>
       <c r="J16" s="30"/>
       <c r="K16" s="43"/>
-      <c r="L16" t="s">
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="U16" t="s">
         <v>280</v>
       </c>
-      <c r="N16">
-        <f>(N7*10)-(N15*2)</f>
+      <c r="W16">
+        <f>(W7*10)-(W15*2)</f>
         <v>616</v>
       </c>
-      <c r="O16">
-        <f>ROUNDUP(N16/10,0)</f>
+      <c r="X16">
+        <f>ROUNDUP(W16/10,0)</f>
         <v>62</v>
       </c>
-      <c r="P16">
+      <c r="Y16">
         <v>4</v>
       </c>
-      <c r="Q16">
-        <f>O16*P16</f>
+      <c r="Z16">
+        <f>X16*Y16</f>
         <v>248</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="173"/>
+    <row r="17" spans="1:26" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="174"/>
       <c r="B17" s="7" t="s">
         <v>59</v>
       </c>
@@ -5358,21 +5582,34 @@
       <c r="I17" s="15"/>
       <c r="J17" s="31"/>
       <c r="K17" s="43"/>
-      <c r="L17" t="s">
+      <c r="L17" s="182" t="s">
+        <v>304</v>
+      </c>
+      <c r="M17" s="150" t="s">
+        <v>302</v>
+      </c>
+      <c r="N17" s="23">
+        <f>N7+6.5</f>
+        <v>670.5</v>
+      </c>
+      <c r="O17" t="s">
+        <v>305</v>
+      </c>
+      <c r="U17" t="s">
         <v>284</v>
       </c>
-      <c r="O17">
+      <c r="X17">
         <v>13</v>
       </c>
-      <c r="P17">
+      <c r="Y17">
         <v>4</v>
       </c>
-      <c r="Q17">
-        <f>O17*P17</f>
+      <c r="Z17">
+        <f>X17*Y17</f>
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="109" t="s">
         <v>205</v>
       </c>
@@ -5400,19 +5637,30 @@
         <v>5423.9999999999991</v>
       </c>
       <c r="I18" s="104">
-        <f>E18*H18</f>
+        <f t="shared" ref="I18:I23" si="4">E18*H18</f>
         <v>21695.999999999996</v>
       </c>
       <c r="J18" s="106" t="s">
         <v>88</v>
       </c>
       <c r="K18" s="42"/>
-      <c r="Q18">
-        <f>SUM(Q16:Q17)</f>
+      <c r="L18" s="187"/>
+      <c r="M18" s="150" t="s">
+        <v>303</v>
+      </c>
+      <c r="N18" s="23">
+        <f>N8+6.5</f>
+        <v>670.5</v>
+      </c>
+      <c r="O18" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z18">
+        <f>SUM(Z16:Z17)</f>
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="109" t="s">
         <v>238</v>
       </c>
@@ -5436,7 +5684,7 @@
         <v>9900</v>
       </c>
       <c r="I19" s="104">
-        <f>E19*H19</f>
+        <f t="shared" si="4"/>
         <v>9900</v>
       </c>
       <c r="J19" s="134" t="s">
@@ -5444,7 +5692,7 @@
       </c>
       <c r="K19" s="42"/>
     </row>
-    <row r="20" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="109" t="s">
         <v>241</v>
       </c>
@@ -5468,7 +5716,7 @@
         <v>19900</v>
       </c>
       <c r="I20" s="104">
-        <f>E20*H20</f>
+        <f t="shared" si="4"/>
         <v>19900</v>
       </c>
       <c r="J20" s="134" t="s">
@@ -5476,15 +5724,15 @@
       </c>
       <c r="K20" s="42"/>
     </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="171" t="s">
+    <row r="21" spans="1:26" ht="16.5">
+      <c r="A21" s="172" t="s">
         <v>289</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>285</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="183" t="s">
+      <c r="D21" s="169" t="s">
         <v>286</v>
       </c>
       <c r="E21" s="9">
@@ -5496,19 +5744,19 @@
         <v>3710</v>
       </c>
       <c r="I21" s="104">
-        <f>E21*H21</f>
+        <f t="shared" si="4"/>
         <v>14840</v>
       </c>
       <c r="J21" s="138"/>
       <c r="K21" s="41"/>
     </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="172"/>
+    <row r="22" spans="1:26">
+      <c r="A22" s="173"/>
       <c r="B22" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="184"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="9">
         <v>4</v>
       </c>
@@ -5518,19 +5766,19 @@
         <v>1710</v>
       </c>
       <c r="I22" s="104">
-        <f>E22*H22</f>
+        <f t="shared" si="4"/>
         <v>6840</v>
       </c>
       <c r="J22" s="138"/>
       <c r="K22" s="41"/>
     </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="173"/>
+    <row r="23" spans="1:26">
+      <c r="A23" s="174"/>
       <c r="B23" s="9" t="s">
         <v>288</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="185"/>
+      <c r="D23" s="171"/>
       <c r="E23" s="9">
         <v>12</v>
       </c>
@@ -5540,13 +5788,13 @@
         <v>500</v>
       </c>
       <c r="I23" s="104">
-        <f>E23*H23</f>
+        <f t="shared" si="4"/>
         <v>6000</v>
       </c>
       <c r="J23" s="138"/>
       <c r="K23" s="41"/>
     </row>
-    <row r="24" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:26" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="109" t="s">
         <v>292</v>
       </c>
@@ -5566,33 +5814,33 @@
       <c r="I24" s="104"/>
       <c r="J24" s="138"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:26">
       <c r="D25" s="22"/>
     </row>
-    <row r="26" spans="1:17">
-      <c r="B26" s="182"/>
+    <row r="26" spans="1:26">
+      <c r="B26" s="151"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:17">
-      <c r="B27" s="186"/>
-    </row>
-    <row r="28" spans="1:17">
+    <row r="27" spans="1:26">
+      <c r="B27" s="152"/>
+    </row>
+    <row r="28" spans="1:26">
       <c r="B28" s="41"/>
       <c r="I28" s="117">
         <f>SUM(I2:I26)</f>
         <v>113676</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:26">
       <c r="B29" s="41"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:26">
       <c r="B30" s="41"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:26">
       <c r="B31" s="41"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:26">
       <c r="B32" s="41"/>
       <c r="E32" s="4"/>
       <c r="G32" s="4"/>
@@ -5601,14 +5849,23 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4"/>
-      <c r="B33" s="182"/>
+      <c r="B33" s="151"/>
     </row>
     <row r="34" spans="1:2">
       <c r="B34" s="22"/>
     </row>
     <row r="49" ht="16.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="U7:U10"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="L14:L15"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A3:A7"/>
@@ -5616,11 +5873,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5642,7 +5894,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5661,16 +5913,16 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
-    <col min="2" max="2" width="37.625" customWidth="1"/>
-    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.25">
+    <row r="1" spans="1:24" ht="18.75">
       <c r="A1" s="78" t="s">
         <v>170</v>
       </c>
@@ -5688,7 +5940,7 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="182" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="72" t="s">
@@ -5697,10 +5949,10 @@
       <c r="C2" s="29">
         <v>4</v>
       </c>
-      <c r="D2" s="178">
+      <c r="D2" s="184">
         <v>4</v>
       </c>
-      <c r="E2" s="178">
+      <c r="E2" s="184">
         <v>6</v>
       </c>
       <c r="H2" s="143">
@@ -5753,15 +6005,15 @@
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="177"/>
+      <c r="A3" s="183"/>
       <c r="B3" s="72" t="s">
         <v>164</v>
       </c>
       <c r="C3" s="29">
         <v>2</v>
       </c>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
+      <c r="D3" s="185"/>
+      <c r="E3" s="185"/>
       <c r="H3" s="143" t="s">
         <v>258</v>
       </c>
@@ -5804,15 +6056,15 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="177"/>
+      <c r="A4" s="183"/>
       <c r="B4" s="83" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="179"/>
-      <c r="E4" s="179"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
       <c r="H4" s="139" t="s">
         <v>263</v>
       </c>
@@ -5856,29 +6108,29 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="177"/>
+      <c r="A5" s="183"/>
       <c r="B5" s="84" t="s">
         <v>219</v>
       </c>
       <c r="C5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="179"/>
-      <c r="E5" s="179"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
       <c r="N5" s="142" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="177"/>
+      <c r="A6" s="183"/>
       <c r="B6" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C6" s="70">
         <v>1</v>
       </c>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
       <c r="H6" s="139" t="s">
         <v>275</v>
       </c>
@@ -5887,18 +6139,18 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="177"/>
+      <c r="A7" s="183"/>
       <c r="B7" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C7" s="70">
         <v>1</v>
       </c>
-      <c r="D7" s="179"/>
-      <c r="E7" s="179"/>
+      <c r="D7" s="185"/>
+      <c r="E7" s="185"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="182" t="s">
         <v>166</v>
       </c>
       <c r="B8" s="83" t="s">
@@ -5907,23 +6159,23 @@
       <c r="C8" s="71">
         <v>1</v>
       </c>
-      <c r="D8" s="178">
+      <c r="D8" s="184">
         <v>2</v>
       </c>
-      <c r="E8" s="178">
+      <c r="E8" s="184">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="177"/>
+      <c r="A9" s="183"/>
       <c r="B9" s="74" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="71">
         <v>1</v>
       </c>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="185"/>
       <c r="H9" t="s">
         <v>222</v>
       </c>
@@ -5945,15 +6197,15 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="181"/>
+      <c r="A10" s="187"/>
       <c r="B10" s="75" t="s">
         <v>167</v>
       </c>
       <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
+      <c r="D10" s="186"/>
+      <c r="E10" s="186"/>
       <c r="H10" t="s">
         <v>178</v>
       </c>
@@ -6090,7 +6342,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="46" spans="1:1">
       <c r="A46" s="22" t="s">
@@ -6115,7 +6367,7 @@
       <selection activeCell="AJ38" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="54" spans="1:1">
       <c r="A54" s="22" t="s">
@@ -6140,7 +6392,7 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="55" spans="1:1">
       <c r="A55" s="22" t="s">
@@ -6165,7 +6417,7 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="22" t="s">

</xml_diff>

<commit_message>
z height adjusted to 140
</commit_message>
<xml_diff>
--- a/doc/parts.xlsx
+++ b/doc/parts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\Mostly-Printed-CNC\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\03.Mostly-Printed-CNC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="307">
   <si>
     <t>QTY</t>
   </si>
@@ -1194,22 +1194,26 @@
   <si>
     <t>min</t>
   </si>
+  <si>
+    <t>~250</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="166" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="167" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+    <numFmt numFmtId="179" formatCode="[$₩-412]#,##0;[Red]\-[$₩-412]#,##0"/>
   </numFmts>
   <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1238,14 +1242,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1266,7 +1270,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1275,7 +1279,7 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1284,7 +1288,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1322,14 +1326,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1344,7 +1348,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1352,7 +1356,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1360,7 +1364,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1368,7 +1372,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1376,14 +1380,14 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1654,7 +1658,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1694,19 +1698,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1718,7 +1722,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
@@ -1766,7 +1770,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1775,7 +1779,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1859,7 +1863,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1895,7 +1899,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1967,7 +1971,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2006,10 +2010,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2018,22 +2022,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2051,10 +2055,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2114,6 +2118,39 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2123,15 +2160,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2147,20 +2175,35 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2186,24 +2229,6 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2216,31 +2241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2752,7 +2759,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3020,16 +3027,16 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" customWidth="1"/>
+    <col min="2" max="2" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="41.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3067,7 +3074,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="156" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="69" t="s">
@@ -3099,7 +3106,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A5" s="165"/>
+      <c r="A5" s="157"/>
       <c r="B5" s="48" t="s">
         <v>77</v>
       </c>
@@ -3129,7 +3136,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A6" s="166" t="s">
+      <c r="A6" s="158" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="53" t="s">
@@ -3161,7 +3168,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A7" s="167"/>
+      <c r="A7" s="159"/>
       <c r="B7" s="53" t="s">
         <v>7</v>
       </c>
@@ -3191,7 +3198,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A8" s="168"/>
+      <c r="A8" s="160"/>
       <c r="B8" s="53" t="s">
         <v>8</v>
       </c>
@@ -3221,7 +3228,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="161" t="s">
         <v>154</v>
       </c>
       <c r="B9" s="48" t="s">
@@ -3253,7 +3260,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A10" s="157"/>
+      <c r="A10" s="162"/>
       <c r="B10" s="48" t="s">
         <v>10</v>
       </c>
@@ -3283,7 +3290,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A11" s="157"/>
+      <c r="A11" s="162"/>
       <c r="B11" s="48" t="s">
         <v>11</v>
       </c>
@@ -3313,7 +3320,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A12" s="158"/>
+      <c r="A12" s="163"/>
       <c r="B12" s="48" t="s">
         <v>17</v>
       </c>
@@ -3343,7 +3350,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="158" t="s">
         <v>155</v>
       </c>
       <c r="B13" s="53" t="s">
@@ -3375,7 +3382,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A14" s="167"/>
+      <c r="A14" s="159"/>
       <c r="B14" s="53" t="s">
         <v>16</v>
       </c>
@@ -3405,7 +3412,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A15" s="167"/>
+      <c r="A15" s="159"/>
       <c r="B15" s="53" t="s">
         <v>123</v>
       </c>
@@ -3435,7 +3442,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A16" s="167"/>
+      <c r="A16" s="159"/>
       <c r="B16" s="60" t="s">
         <v>19</v>
       </c>
@@ -3460,7 +3467,7 @@
       <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A17" s="168"/>
+      <c r="A17" s="160"/>
       <c r="B17" s="53" t="s">
         <v>119</v>
       </c>
@@ -3481,7 +3488,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A18" s="156" t="s">
+      <c r="A18" s="161" t="s">
         <v>156</v>
       </c>
       <c r="B18" s="48" t="s">
@@ -3513,7 +3520,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A19" s="158"/>
+      <c r="A19" s="163"/>
       <c r="B19" s="48" t="s">
         <v>74</v>
       </c>
@@ -3543,7 +3550,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A20" s="153" t="s">
+      <c r="A20" s="164" t="s">
         <v>149</v>
       </c>
       <c r="B20" s="88" t="s">
@@ -3571,7 +3578,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A21" s="154"/>
+      <c r="A21" s="165"/>
       <c r="B21" s="88" t="s">
         <v>191</v>
       </c>
@@ -3597,8 +3604,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A22" s="154"/>
-      <c r="B22" s="153" t="s">
+      <c r="A22" s="165"/>
+      <c r="B22" s="164" t="s">
         <v>194</v>
       </c>
       <c r="C22" s="88">
@@ -3623,8 +3630,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A23" s="154"/>
-      <c r="B23" s="154"/>
+      <c r="A23" s="165"/>
+      <c r="B23" s="165"/>
       <c r="C23" s="88">
         <v>1</v>
       </c>
@@ -3647,8 +3654,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A24" s="154"/>
-      <c r="B24" s="155"/>
+      <c r="A24" s="165"/>
+      <c r="B24" s="166"/>
       <c r="C24" s="88">
         <v>1</v>
       </c>
@@ -3671,7 +3678,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A25" s="154"/>
+      <c r="A25" s="165"/>
       <c r="B25" s="88" t="s">
         <v>250</v>
       </c>
@@ -3697,8 +3704,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A26" s="154"/>
-      <c r="B26" s="153" t="s">
+      <c r="A26" s="165"/>
+      <c r="B26" s="164" t="s">
         <v>251</v>
       </c>
       <c r="C26" s="88">
@@ -3707,7 +3714,7 @@
       <c r="D26" s="89">
         <v>0.5</v>
       </c>
-      <c r="E26" s="161" t="s">
+      <c r="E26" s="169" t="s">
         <v>106</v>
       </c>
       <c r="F26" s="88"/>
@@ -3723,15 +3730,15 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A27" s="154"/>
-      <c r="B27" s="154"/>
+      <c r="A27" s="165"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="88">
         <v>1</v>
       </c>
       <c r="D27" s="89">
         <v>0.5</v>
       </c>
-      <c r="E27" s="162"/>
+      <c r="E27" s="170"/>
       <c r="F27" s="88"/>
       <c r="G27" s="57"/>
       <c r="H27" s="100" t="s">
@@ -3745,15 +3752,15 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A28" s="155"/>
-      <c r="B28" s="155"/>
+      <c r="A28" s="166"/>
+      <c r="B28" s="166"/>
       <c r="C28" s="88">
         <v>1</v>
       </c>
       <c r="D28" s="89">
         <v>0.5</v>
       </c>
-      <c r="E28" s="163"/>
+      <c r="E28" s="171"/>
       <c r="F28" s="88"/>
       <c r="G28" s="57"/>
       <c r="H28" s="100" t="s">
@@ -3767,7 +3774,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A29" s="156" t="s">
+      <c r="A29" s="161" t="s">
         <v>162</v>
       </c>
       <c r="B29" s="90" t="s">
@@ -3797,7 +3804,7 @@
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A30" s="157"/>
+      <c r="A30" s="162"/>
       <c r="B30" s="48" t="s">
         <v>159</v>
       </c>
@@ -3825,8 +3832,8 @@
       <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A31" s="157"/>
-      <c r="B31" s="156" t="s">
+      <c r="A31" s="162"/>
+      <c r="B31" s="161" t="s">
         <v>158</v>
       </c>
       <c r="C31" s="47">
@@ -3853,8 +3860,8 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A32" s="157"/>
-      <c r="B32" s="158"/>
+      <c r="A32" s="162"/>
+      <c r="B32" s="163"/>
       <c r="C32" s="47">
         <v>1</v>
       </c>
@@ -3879,8 +3886,8 @@
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A33" s="157"/>
-      <c r="B33" s="156" t="s">
+      <c r="A33" s="162"/>
+      <c r="B33" s="161" t="s">
         <v>161</v>
       </c>
       <c r="C33" s="47">
@@ -3889,7 +3896,7 @@
       <c r="D33" s="49">
         <v>0.7</v>
       </c>
-      <c r="E33" s="159" t="s">
+      <c r="E33" s="167" t="s">
         <v>106</v>
       </c>
       <c r="F33" s="47"/>
@@ -3903,15 +3910,15 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A34" s="157"/>
-      <c r="B34" s="157"/>
+      <c r="A34" s="162"/>
+      <c r="B34" s="162"/>
       <c r="C34" s="47">
         <v>1</v>
       </c>
       <c r="D34" s="49">
         <v>0.7</v>
       </c>
-      <c r="E34" s="160"/>
+      <c r="E34" s="168"/>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
       <c r="H34" s="97" t="s">
@@ -3927,8 +3934,8 @@
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A35" s="157"/>
-      <c r="B35" s="158"/>
+      <c r="A35" s="162"/>
+      <c r="B35" s="163"/>
       <c r="C35" s="47">
         <v>1</v>
       </c>
@@ -3949,8 +3956,8 @@
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A36" s="157"/>
-      <c r="B36" s="156" t="s">
+      <c r="A36" s="162"/>
+      <c r="B36" s="161" t="s">
         <v>160</v>
       </c>
       <c r="C36" s="47">
@@ -3959,7 +3966,7 @@
       <c r="D36" s="49">
         <v>0.7</v>
       </c>
-      <c r="E36" s="159" t="s">
+      <c r="E36" s="167" t="s">
         <v>106</v>
       </c>
       <c r="F36" s="47"/>
@@ -3970,15 +3977,15 @@
       <c r="I36" s="52"/>
     </row>
     <row r="37" spans="1:12" ht="28.5" customHeight="1">
-      <c r="A37" s="158"/>
-      <c r="B37" s="158"/>
+      <c r="A37" s="163"/>
+      <c r="B37" s="163"/>
       <c r="C37" s="47">
         <v>1</v>
       </c>
       <c r="D37" s="49">
         <v>0.7</v>
       </c>
-      <c r="E37" s="160"/>
+      <c r="E37" s="168"/>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
       <c r="H37" s="97" t="s">
@@ -4033,11 +4040,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A13:A17"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="A29:A37"/>
     <mergeCell ref="E33:E34"/>
@@ -4048,6 +4050,11 @@
     <mergeCell ref="A20:A28"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="E26:E28"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A13:A17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -4095,15 +4102,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="121.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.100000000000001" customHeight="1">
@@ -4642,7 +4649,7 @@
         <v>31536</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="21">
+    <row r="32" spans="1:9" ht="26.25">
       <c r="D32" s="131" t="s">
         <v>217</v>
       </c>
@@ -4688,31 +4695,31 @@
   </sheetPr>
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="107.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="107.625" customWidth="1"/>
+    <col min="5" max="5" width="8.125" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="7.75" customWidth="1"/>
+    <col min="15" max="15" width="4.25" customWidth="1"/>
+    <col min="16" max="16" width="5.625" customWidth="1"/>
     <col min="17" max="17" width="7" customWidth="1"/>
-    <col min="25" max="25" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" customWidth="1"/>
+    <col min="25" max="25" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="20.100000000000001" customHeight="1">
@@ -4786,7 +4793,7 @@
       <c r="K2" s="43"/>
       <c r="L2" s="23"/>
       <c r="M2" s="150"/>
-      <c r="N2" s="189" t="s">
+      <c r="N2" s="154" t="s">
         <v>296</v>
       </c>
       <c r="U2" s="23"/>
@@ -4799,7 +4806,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="172" t="s">
+      <c r="A3" s="185" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="34" t="s">
@@ -4838,7 +4845,7 @@
       <c r="M3" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="194">
         <v>400</v>
       </c>
       <c r="U3" s="177" t="s">
@@ -4856,7 +4863,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="173"/>
+      <c r="A4" s="186"/>
       <c r="B4" s="6" t="s">
         <v>46</v>
       </c>
@@ -4889,7 +4896,7 @@
       <c r="M4" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="194">
         <v>400</v>
       </c>
       <c r="U4" s="178"/>
@@ -4905,7 +4912,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="173"/>
+      <c r="A5" s="186"/>
       <c r="B5" s="6" t="s">
         <v>48</v>
       </c>
@@ -4938,8 +4945,8 @@
       <c r="M5" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="N5" s="23">
-        <v>150</v>
+      <c r="N5" s="194">
+        <v>140</v>
       </c>
       <c r="U5" s="178"/>
       <c r="V5" s="19" t="s">
@@ -4954,7 +4961,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="173"/>
+      <c r="A6" s="186"/>
       <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
@@ -4992,7 +4999,7 @@
       <c r="X6" s="24"/>
     </row>
     <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="174"/>
+      <c r="A7" s="187"/>
       <c r="B7" s="7" t="s">
         <v>52</v>
       </c>
@@ -5028,7 +5035,7 @@
       <c r="M7" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="193">
+      <c r="N7" s="155">
         <f>N3+264</f>
         <v>664</v>
       </c>
@@ -5039,7 +5046,7 @@
         <f>N7*P7</f>
         <v>1992</v>
       </c>
-      <c r="U7" s="190" t="s">
+      <c r="U7" s="174" t="s">
         <v>99</v>
       </c>
       <c r="V7" s="19" t="s">
@@ -5062,7 +5069,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="175" t="s">
+      <c r="A8" s="188" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="35" t="s">
@@ -5099,7 +5106,7 @@
       <c r="M8" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="N8" s="193">
+      <c r="N8" s="155">
         <f>N4+264</f>
         <v>664</v>
       </c>
@@ -5110,7 +5117,7 @@
         <f>N8*P8</f>
         <v>1992</v>
       </c>
-      <c r="U8" s="191"/>
+      <c r="U8" s="175"/>
       <c r="V8" s="19" t="s">
         <v>96</v>
       </c>
@@ -5131,7 +5138,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="176"/>
+      <c r="A9" s="189"/>
       <c r="B9" s="38" t="s">
         <v>139</v>
       </c>
@@ -5166,22 +5173,18 @@
       <c r="M9" s="150" t="s">
         <v>92</v>
       </c>
-      <c r="N9" s="193">
+      <c r="N9" s="155">
         <f>N5+190</f>
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
       <c r="Q9">
         <f>N9*P9</f>
-        <v>680</v>
-      </c>
-      <c r="S9">
-        <f>W9*10-N9</f>
-        <v>110</v>
-      </c>
-      <c r="U9" s="191"/>
+        <v>660</v>
+      </c>
+      <c r="U9" s="175"/>
       <c r="V9" s="19" t="s">
         <v>97</v>
       </c>
@@ -5202,7 +5205,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="172" t="s">
+      <c r="A10" s="185" t="s">
         <v>147</v>
       </c>
       <c r="B10" s="34" t="s">
@@ -5240,22 +5243,18 @@
       <c r="M10" s="150" t="s">
         <v>299</v>
       </c>
-      <c r="N10" s="193">
+      <c r="N10" s="155">
         <f>N5-13</f>
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="P10">
         <v>4</v>
       </c>
       <c r="Q10">
         <f>N10*P10</f>
-        <v>548</v>
-      </c>
-      <c r="S10">
-        <f>W10*10-N10</f>
-        <v>113</v>
-      </c>
-      <c r="U10" s="192"/>
+        <v>508</v>
+      </c>
+      <c r="U10" s="176"/>
       <c r="V10" s="25" t="s">
         <v>283</v>
       </c>
@@ -5272,7 +5271,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="173"/>
+      <c r="A11" s="186"/>
       <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
@@ -5303,7 +5302,7 @@
       <c r="K11" s="43"/>
       <c r="Q11">
         <f>SUM(Q7:Q10)</f>
-        <v>5212</v>
+        <v>5152</v>
       </c>
       <c r="Z11">
         <f>SUM(Z7:Z10)</f>
@@ -5311,7 +5310,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="174"/>
+      <c r="A12" s="187"/>
       <c r="B12" s="7" t="s">
         <v>66</v>
       </c>
@@ -5346,17 +5345,15 @@
       <c r="M12" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="N12" s="193">
+      <c r="N12" s="155">
         <f>N5+76</f>
-        <v>226</v>
-      </c>
-      <c r="O12" s="188" t="s">
+        <v>216</v>
+      </c>
+      <c r="O12" s="153" t="s">
         <v>305</v>
       </c>
-      <c r="P12" s="4"/>
-      <c r="S12">
-        <f>W12*10-N12</f>
-        <v>173.20000000000005</v>
+      <c r="P12" s="153" t="s">
+        <v>306</v>
       </c>
       <c r="U12" s="19" t="s">
         <v>100</v>
@@ -5374,7 +5371,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="172" t="s">
+      <c r="A13" s="185" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="34" t="s">
@@ -5411,7 +5408,7 @@
       <c r="M13" s="105"/>
     </row>
     <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="173"/>
+      <c r="A14" s="186"/>
       <c r="B14" s="6" t="s">
         <v>62</v>
       </c>
@@ -5440,7 +5437,7 @@
         <v>88</v>
       </c>
       <c r="K14" s="43"/>
-      <c r="L14" s="182" t="s">
+      <c r="L14" s="172" t="s">
         <v>301</v>
       </c>
       <c r="M14" s="25" t="s">
@@ -5468,7 +5465,7 @@
       <c r="Z14" s="105"/>
     </row>
     <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="174"/>
+      <c r="A15" s="187"/>
       <c r="B15" s="7" t="s">
         <v>64</v>
       </c>
@@ -5497,7 +5494,7 @@
         <v>88</v>
       </c>
       <c r="K15" s="43"/>
-      <c r="L15" s="187"/>
+      <c r="L15" s="173"/>
       <c r="M15" s="150" t="s">
         <v>303</v>
       </c>
@@ -5520,7 +5517,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="172" t="s">
+      <c r="A16" s="185" t="s">
         <v>149</v>
       </c>
       <c r="B16" s="34" t="s">
@@ -5563,7 +5560,7 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="174"/>
+      <c r="A17" s="187"/>
       <c r="B17" s="7" t="s">
         <v>59</v>
       </c>
@@ -5582,7 +5579,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="31"/>
       <c r="K17" s="43"/>
-      <c r="L17" s="182" t="s">
+      <c r="L17" s="172" t="s">
         <v>304</v>
       </c>
       <c r="M17" s="150" t="s">
@@ -5644,7 +5641,7 @@
         <v>88</v>
       </c>
       <c r="K18" s="42"/>
-      <c r="L18" s="187"/>
+      <c r="L18" s="173"/>
       <c r="M18" s="150" t="s">
         <v>303</v>
       </c>
@@ -5724,15 +5721,15 @@
       </c>
       <c r="K20" s="42"/>
     </row>
-    <row r="21" spans="1:26" ht="16.5">
-      <c r="A21" s="172" t="s">
+    <row r="21" spans="1:26">
+      <c r="A21" s="185" t="s">
         <v>289</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>285</v>
       </c>
       <c r="C21" s="9"/>
-      <c r="D21" s="169" t="s">
+      <c r="D21" s="182" t="s">
         <v>286</v>
       </c>
       <c r="E21" s="9">
@@ -5751,12 +5748,12 @@
       <c r="K21" s="41"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="173"/>
+      <c r="A22" s="186"/>
       <c r="B22" s="9" t="s">
         <v>287</v>
       </c>
       <c r="C22" s="9"/>
-      <c r="D22" s="170"/>
+      <c r="D22" s="183"/>
       <c r="E22" s="9">
         <v>4</v>
       </c>
@@ -5773,12 +5770,12 @@
       <c r="K22" s="41"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="174"/>
+      <c r="A23" s="187"/>
       <c r="B23" s="9" t="s">
         <v>288</v>
       </c>
       <c r="C23" s="9"/>
-      <c r="D23" s="171"/>
+      <c r="D23" s="184"/>
       <c r="E23" s="9">
         <v>12</v>
       </c>
@@ -5857,6 +5854,13 @@
     <row r="49" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="U7:U10"/>
     <mergeCell ref="U3:U5"/>
@@ -5866,13 +5870,6 @@
     <mergeCell ref="L3:L5"/>
     <mergeCell ref="L7:L10"/>
     <mergeCell ref="L14:L15"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5894,7 +5891,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5913,16 +5910,16 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="37.625" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18.75">
+    <row r="1" spans="1:24" ht="20.25">
       <c r="A1" s="78" t="s">
         <v>170</v>
       </c>
@@ -5940,7 +5937,7 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" s="182" t="s">
+      <c r="A2" s="172" t="s">
         <v>165</v>
       </c>
       <c r="B2" s="72" t="s">
@@ -5949,10 +5946,10 @@
       <c r="C2" s="29">
         <v>4</v>
       </c>
-      <c r="D2" s="184">
+      <c r="D2" s="191">
         <v>4</v>
       </c>
-      <c r="E2" s="184">
+      <c r="E2" s="191">
         <v>6</v>
       </c>
       <c r="H2" s="143">
@@ -6005,15 +6002,15 @@
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" s="183"/>
+      <c r="A3" s="190"/>
       <c r="B3" s="72" t="s">
         <v>164</v>
       </c>
       <c r="C3" s="29">
         <v>2</v>
       </c>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
       <c r="H3" s="143" t="s">
         <v>258</v>
       </c>
@@ -6056,15 +6053,15 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="183"/>
+      <c r="A4" s="190"/>
       <c r="B4" s="83" t="s">
         <v>218</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="185"/>
-      <c r="E4" s="185"/>
+      <c r="D4" s="192"/>
+      <c r="E4" s="192"/>
       <c r="H4" s="139" t="s">
         <v>263</v>
       </c>
@@ -6108,29 +6105,29 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="183"/>
+      <c r="A5" s="190"/>
       <c r="B5" s="84" t="s">
         <v>219</v>
       </c>
       <c r="C5" s="29">
         <v>1</v>
       </c>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="192"/>
       <c r="N5" s="142" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" s="183"/>
+      <c r="A6" s="190"/>
       <c r="B6" s="81" t="s">
         <v>221</v>
       </c>
       <c r="C6" s="70">
         <v>1</v>
       </c>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
       <c r="H6" s="139" t="s">
         <v>275</v>
       </c>
@@ -6139,18 +6136,18 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="183"/>
+      <c r="A7" s="190"/>
       <c r="B7" s="73" t="s">
         <v>175</v>
       </c>
       <c r="C7" s="70">
         <v>1</v>
       </c>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="182" t="s">
+      <c r="A8" s="172" t="s">
         <v>166</v>
       </c>
       <c r="B8" s="83" t="s">
@@ -6159,23 +6156,23 @@
       <c r="C8" s="71">
         <v>1</v>
       </c>
-      <c r="D8" s="184">
+      <c r="D8" s="191">
         <v>2</v>
       </c>
-      <c r="E8" s="184">
+      <c r="E8" s="191">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" s="183"/>
+      <c r="A9" s="190"/>
       <c r="B9" s="74" t="s">
         <v>175</v>
       </c>
       <c r="C9" s="71">
         <v>1</v>
       </c>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
+      <c r="D9" s="192"/>
+      <c r="E9" s="192"/>
       <c r="H9" t="s">
         <v>222</v>
       </c>
@@ -6197,15 +6194,15 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="187"/>
+      <c r="A10" s="173"/>
       <c r="B10" s="75" t="s">
         <v>167</v>
       </c>
       <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
       <c r="H10" t="s">
         <v>178</v>
       </c>
@@ -6342,7 +6339,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="46" spans="1:1">
       <c r="A46" s="22" t="s">
@@ -6367,7 +6364,7 @@
       <selection activeCell="AJ38" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="54" spans="1:1">
       <c r="A54" s="22" t="s">
@@ -6392,7 +6389,7 @@
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="55" spans="1:1">
       <c r="A55" s="22" t="s">
@@ -6417,7 +6414,7 @@
       <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="22" t="s">

</xml_diff>